<commit_message>
Added a save round and load round button along with persistent save in browser, export to excel button doesn't work
</commit_message>
<xml_diff>
--- a/Data/Draft Files/PMI Provided Course List Edits.xlsx
+++ b/Data/Draft Files/PMI Provided Course List Edits.xlsx
@@ -5,13 +5,13 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\SchedulePro\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\SchedulePro\Data\Draft Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:2001_{00BFEE1B-D5A2-4C37-91B4-7E31FA584822}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0F4634-8A5F-40BF-9DD4-5CD198C62002}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="882" activeTab="11" xr2:uid="{E7EE0092-2BA9-4A50-8785-723FB1934021}"/>
-    <workbookView xWindow="-52635" yWindow="1905" windowWidth="23010" windowHeight="12210" tabRatio="803" firstSheet="1" activeTab="7" xr2:uid="{9F697EAD-8F97-428C-B497-BADBFF50374A}"/>
+    <workbookView xWindow="-53445" yWindow="2265" windowWidth="23010" windowHeight="12210" tabRatio="882" activeTab="11" xr2:uid="{E7EE0092-2BA9-4A50-8785-723FB1934021}"/>
+    <workbookView xWindow="-53010" yWindow="2700" windowWidth="23010" windowHeight="12210" tabRatio="803" firstSheet="3" activeTab="10" xr2:uid="{9F697EAD-8F97-428C-B497-BADBFF50374A}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Data" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,6 @@
     <sheet name="Important Notes" sheetId="6" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -419,7 +418,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -441,7 +440,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5081" uniqueCount="511">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5088" uniqueCount="518">
   <si>
     <t>Month</t>
   </si>
@@ -1992,6 +1991,27 @@
   </si>
   <si>
     <t>tyson rydl has two courses with basically same name - are they different day durations?</t>
+  </si>
+  <si>
+    <t>round publishing with incremental numbering and loading</t>
+  </si>
+  <si>
+    <t>buttons could use some cleaning</t>
+  </si>
+  <si>
+    <t>events and event days more interactive within dashboard - perhaps add, remove, and change names</t>
+  </si>
+  <si>
+    <t>Should be able to change course names in app - logged as change</t>
+  </si>
+  <si>
+    <t>Next steps</t>
+  </si>
+  <si>
+    <t>Room numbers per swimlane. Same page as configure rooms</t>
+  </si>
+  <si>
+    <t>notes will be crucial for example half day saying 9 am to 1 pm</t>
   </si>
 </sst>
 </file>
@@ -2445,7 +2465,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="264">
+  <cellXfs count="263">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3086,9 +3106,8 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -3100,16 +3119,16 @@
   <dxfs count="19">
     <dxf>
       <border outline="0">
-        <bottom style="thin">
+        <top style="thin">
           <color rgb="FF44B3E1"/>
-        </bottom>
+        </top>
       </border>
     </dxf>
     <dxf>
       <border outline="0">
-        <top style="thin">
+        <bottom style="thin">
           <color rgb="FF44B3E1"/>
-        </top>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -3137,6 +3156,20 @@
       </fill>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3157,44 +3190,6 @@
         <patternFill patternType="solid">
           <fgColor theme="4"/>
           <bgColor theme="4"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor auto="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3369,6 +3364,60 @@
       </border>
     </dxf>
     <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </left>
+        <right style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </right>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor auto="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -3391,36 +3440,6 @@
           <bgColor theme="4"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <left style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </left>
-        <right style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </right>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -4297,24 +4316,24 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0B17CE91-6F2D-4FD9-BD14-C2F10C47A727}" name="Table4" displayName="Table4" ref="A1:E157" totalsRowShown="0" headerRowDxfId="12" dataDxfId="6" headerRowBorderDxfId="14" tableBorderDxfId="15" totalsRowBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{0B17CE91-6F2D-4FD9-BD14-C2F10C47A727}" name="Table4" displayName="Table4" ref="A1:E157" totalsRowShown="0" headerRowDxfId="15" dataDxfId="13" headerRowBorderDxfId="14" tableBorderDxfId="12" totalsRowBorderDxfId="11">
   <autoFilter ref="A1:E157" xr:uid="{0B17CE91-6F2D-4FD9-BD14-C2F10C47A727}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E157">
     <sortCondition ref="A1:A157"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{300C4B56-6AD2-498F-A5EC-0B1C27527F78}" name="Course_ID" dataDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{CA628A62-9D0D-4F06-BA32-ED1B78D9E7CB}" name="Instructor" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{8FD134A2-0E04-464D-89DE-DF6CA9229D48}" name="Course_Name" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{3188DD13-718A-42E4-A064-BF3D7A9C4D81}" name="Duration_Days" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{4C4A1C66-1BA5-43A2-B99F-82EF17F83843}" name="TOPIC" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{300C4B56-6AD2-498F-A5EC-0B1C27527F78}" name="Course_ID" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{CA628A62-9D0D-4F06-BA32-ED1B78D9E7CB}" name="Instructor" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{8FD134A2-0E04-464D-89DE-DF6CA9229D48}" name="Course_Name" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{3188DD13-718A-42E4-A064-BF3D7A9C4D81}" name="Duration_Days" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{4C4A1C66-1BA5-43A2-B99F-82EF17F83843}" name="TOPIC" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C5A64D9E-65A6-4F63-94E6-0A6CE0063594}" name="Table6" displayName="Table6" ref="A1:E104" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="4" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C5A64D9E-65A6-4F63-94E6-0A6CE0063594}" name="Table6" displayName="Table6" ref="A1:E104" totalsRowShown="0" headerRowDxfId="5" headerRowBorderDxfId="4" tableBorderDxfId="3">
   <autoFilter ref="A1:E104" xr:uid="{C5A64D9E-65A6-4F63-94E6-0A6CE0063594}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E104">
     <sortCondition ref="B1:B104"/>
@@ -4331,7 +4350,7 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DB961DDC-9553-424B-B5B3-C6BC7EBF15D9}" name="Table68" displayName="Table68" ref="A1:G104" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="0" tableBorderDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{DB961DDC-9553-424B-B5B3-C6BC7EBF15D9}" name="Table68" displayName="Table68" ref="A1:G104" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
   <autoFilter ref="A1:G104" xr:uid="{C5A64D9E-65A6-4F63-94E6-0A6CE0063594}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E104">
     <sortCondition ref="B1:B104"/>
@@ -4904,7 +4923,7 @@
     <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
-    <sheetView topLeftCell="M239" workbookViewId="1">
+    <sheetView topLeftCell="C1" workbookViewId="1">
       <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
@@ -18963,7 +18982,7 @@
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="258" t="str">
+      <c r="A20" t="str">
         <v>Managing the Human Side of Projects</v>
       </c>
     </row>
@@ -18973,7 +18992,7 @@
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="258" t="str">
+      <c r="A22" t="str">
         <v>Value Management – Designed, Built, and Operationalized for Success</v>
       </c>
     </row>
@@ -19103,52 +19122,52 @@
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="258" t="str">
+      <c r="A48" t="str">
         <v>Adaptive Project Management</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="258" t="str">
+      <c r="A49" t="str">
         <v>Thrive in the AI Era: Future-Ready PM Skills</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="258" t="str">
+      <c r="A50" t="str">
         <v>Enterprise Risk Management: Master Complex Projects</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="258" t="str">
+      <c r="A51" t="str">
         <v>Cognitive Diversity: Leverage Your Thinking Style</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="258" t="str">
+      <c r="A52" t="str">
         <v>AI for Strategic Decisions: Leveraging Analysis</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="258" t="str">
+      <c r="A53" t="str">
         <v>Next-Gen PMO: Build for Uncertainty</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="258" t="str">
+      <c r="A54" t="str">
         <v>Artificial Intelligence-Powered Project Excellence: Roadmaps, Success Strategies, and Practical Tools</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="258" t="str">
+      <c r="A55" t="str">
         <v>The Engaged, Empowered, and Happy Stakeholder </v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="258" t="str">
+      <c r="A56" t="str">
         <v>Power Skills: Lead, Influence, and Navigate</v>
       </c>
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="258" t="str">
+      <c r="A57" t="str">
         <v>Artificial Intelligence Applied Skills: Unlocking Project Automation and Efficiency Gains</v>
       </c>
     </row>
@@ -19387,13 +19406,13 @@
   <sheetPr codeName="Sheet11">
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="T38" sqref="T38"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19406,6 +19425,41 @@
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>508</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>511</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>515</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>516</v>
       </c>
     </row>
   </sheetData>
@@ -19424,7 +19478,7 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
     <sheetView workbookViewId="1">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19460,17 +19514,17 @@
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" s="258" t="s">
+      <c r="A7" t="s">
         <v>450</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" s="258" t="s">
+      <c r="A8" t="s">
         <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" s="258" t="s">
+      <c r="A9" t="s">
         <v>510</v>
       </c>
     </row>
@@ -29948,19 +30002,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="259" t="s">
+      <c r="A2" s="258" t="s">
         <v>294</v>
       </c>
-      <c r="B2" s="259" t="s">
+      <c r="B2" s="258" t="s">
         <v>76</v>
       </c>
-      <c r="C2" s="259" t="s">
+      <c r="C2" s="258" t="s">
         <v>295</v>
       </c>
-      <c r="D2" s="259">
+      <c r="D2" s="258">
         <v>4</v>
       </c>
-      <c r="E2" s="259" t="s">
+      <c r="E2" s="258" t="s">
         <v>296</v>
       </c>
       <c r="G2" t="str">
@@ -29980,19 +30034,19 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="259" t="s">
+      <c r="A3" s="258" t="s">
         <v>139</v>
       </c>
-      <c r="B3" s="259" t="s">
+      <c r="B3" s="258" t="s">
         <v>141</v>
       </c>
-      <c r="C3" s="259" t="s">
+      <c r="C3" s="258" t="s">
         <v>140</v>
       </c>
-      <c r="D3" s="259">
-        <v>2</v>
-      </c>
-      <c r="E3" s="259" t="s">
+      <c r="D3" s="258">
+        <v>2</v>
+      </c>
+      <c r="E3" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G3" t="str">
@@ -30012,19 +30066,19 @@
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A4" s="259" t="s">
+      <c r="A4" s="258" t="s">
         <v>139</v>
       </c>
-      <c r="B4" s="259" t="s">
+      <c r="B4" s="258" t="s">
         <v>141</v>
       </c>
-      <c r="C4" s="259" t="s">
+      <c r="C4" s="258" t="s">
         <v>140</v>
       </c>
-      <c r="D4" s="259">
-        <v>2</v>
-      </c>
-      <c r="E4" s="259" t="s">
+      <c r="D4" s="258">
+        <v>2</v>
+      </c>
+      <c r="E4" s="258" t="s">
         <v>240</v>
       </c>
       <c r="G4" t="str">
@@ -30044,19 +30098,19 @@
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A5" s="259" t="s">
+      <c r="A5" s="258" t="s">
         <v>139</v>
       </c>
-      <c r="B5" s="259" t="s">
+      <c r="B5" s="258" t="s">
         <v>141</v>
       </c>
-      <c r="C5" s="259" t="s">
+      <c r="C5" s="258" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="259">
-        <v>2</v>
-      </c>
-      <c r="E5" s="259" t="s">
+      <c r="D5" s="258">
+        <v>2</v>
+      </c>
+      <c r="E5" s="258" t="s">
         <v>54</v>
       </c>
       <c r="G5" t="str">
@@ -30076,19 +30130,19 @@
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A6" s="259" t="s">
+      <c r="A6" s="258" t="s">
         <v>139</v>
       </c>
-      <c r="B6" s="259" t="s">
+      <c r="B6" s="258" t="s">
         <v>141</v>
       </c>
-      <c r="C6" s="259" t="s">
+      <c r="C6" s="258" t="s">
         <v>140</v>
       </c>
-      <c r="D6" s="259">
-        <v>2</v>
-      </c>
-      <c r="E6" s="259" t="s">
+      <c r="D6" s="258">
+        <v>2</v>
+      </c>
+      <c r="E6" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G6" t="str">
@@ -30108,19 +30162,19 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A7" s="259" t="s">
+      <c r="A7" s="258" t="s">
         <v>143</v>
       </c>
-      <c r="B7" s="259" t="s">
+      <c r="B7" s="258" t="s">
         <v>141</v>
       </c>
-      <c r="C7" s="259" t="s">
+      <c r="C7" s="258" t="s">
         <v>144</v>
       </c>
-      <c r="D7" s="259">
-        <v>2</v>
-      </c>
-      <c r="E7" s="259" t="s">
+      <c r="D7" s="258">
+        <v>2</v>
+      </c>
+      <c r="E7" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G7" t="str">
@@ -30140,19 +30194,19 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A8" s="259" t="s">
+      <c r="A8" s="258" t="s">
         <v>143</v>
       </c>
-      <c r="B8" s="259" t="s">
+      <c r="B8" s="258" t="s">
         <v>141</v>
       </c>
-      <c r="C8" s="259" t="s">
+      <c r="C8" s="258" t="s">
         <v>144</v>
       </c>
-      <c r="D8" s="259">
-        <v>2</v>
-      </c>
-      <c r="E8" s="259" t="s">
+      <c r="D8" s="258">
+        <v>2</v>
+      </c>
+      <c r="E8" s="258" t="s">
         <v>215</v>
       </c>
       <c r="G8" t="str">
@@ -30172,19 +30226,19 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A9" s="259" t="s">
+      <c r="A9" s="258" t="s">
         <v>326</v>
       </c>
-      <c r="B9" s="259" t="s">
+      <c r="B9" s="258" t="s">
         <v>328</v>
       </c>
-      <c r="C9" s="259" t="s">
+      <c r="C9" s="258" t="s">
         <v>327</v>
       </c>
-      <c r="D9" s="259">
-        <v>2</v>
-      </c>
-      <c r="E9" s="259" t="s">
+      <c r="D9" s="258">
+        <v>2</v>
+      </c>
+      <c r="E9" s="258" t="s">
         <v>60</v>
       </c>
       <c r="G9" t="str">
@@ -30204,19 +30258,19 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A10" s="259" t="s">
+      <c r="A10" s="258" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="259" t="s">
+      <c r="B10" s="258" t="s">
         <v>45</v>
       </c>
-      <c r="C10" s="259" t="s">
+      <c r="C10" s="258" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="259">
-        <v>2</v>
-      </c>
-      <c r="E10" s="259" t="s">
+      <c r="D10" s="258">
+        <v>2</v>
+      </c>
+      <c r="E10" s="258" t="s">
         <v>47</v>
       </c>
       <c r="G10" t="str">
@@ -30236,19 +30290,19 @@
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A11" s="259" t="s">
+      <c r="A11" s="258" t="s">
         <v>43</v>
       </c>
-      <c r="B11" s="259" t="s">
+      <c r="B11" s="258" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="259" t="s">
+      <c r="C11" s="258" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="259">
-        <v>2</v>
-      </c>
-      <c r="E11" s="259" t="s">
+      <c r="D11" s="258">
+        <v>2</v>
+      </c>
+      <c r="E11" s="258" t="s">
         <v>426</v>
       </c>
       <c r="G11" t="str">
@@ -30268,19 +30322,19 @@
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A12" s="259" t="s">
+      <c r="A12" s="258" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="259" t="s">
+      <c r="B12" s="258" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="259" t="s">
+      <c r="C12" s="258" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="259">
-        <v>2</v>
-      </c>
-      <c r="E12" s="259" t="s">
+      <c r="D12" s="258">
+        <v>2</v>
+      </c>
+      <c r="E12" s="258" t="s">
         <v>58</v>
       </c>
       <c r="G12" t="str">
@@ -30300,19 +30354,19 @@
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A13" s="259" t="s">
+      <c r="A13" s="258" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="259" t="s">
+      <c r="B13" s="258" t="s">
         <v>57</v>
       </c>
-      <c r="C13" s="259" t="s">
+      <c r="C13" s="258" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="259">
-        <v>2</v>
-      </c>
-      <c r="E13" s="259" t="s">
+      <c r="D13" s="258">
+        <v>2</v>
+      </c>
+      <c r="E13" s="258" t="s">
         <v>240</v>
       </c>
       <c r="G13" t="str">
@@ -30332,19 +30386,19 @@
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A14" s="259" t="s">
+      <c r="A14" s="258" t="s">
         <v>55</v>
       </c>
-      <c r="B14" s="259" t="s">
+      <c r="B14" s="258" t="s">
         <v>57</v>
       </c>
-      <c r="C14" s="259" t="s">
+      <c r="C14" s="258" t="s">
         <v>59</v>
       </c>
-      <c r="D14" s="259">
-        <v>2</v>
-      </c>
-      <c r="E14" s="259" t="s">
+      <c r="D14" s="258">
+        <v>2</v>
+      </c>
+      <c r="E14" s="258" t="s">
         <v>60</v>
       </c>
       <c r="G14" t="str">
@@ -30364,19 +30418,19 @@
       </c>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A15" s="259" t="s">
+      <c r="A15" s="258" t="s">
         <v>124</v>
       </c>
-      <c r="B15" s="259" t="s">
+      <c r="B15" s="258" t="s">
         <v>126</v>
       </c>
-      <c r="C15" s="259" t="s">
+      <c r="C15" s="258" t="s">
         <v>125</v>
       </c>
-      <c r="D15" s="259">
-        <v>2</v>
-      </c>
-      <c r="E15" s="259" t="s">
+      <c r="D15" s="258">
+        <v>2</v>
+      </c>
+      <c r="E15" s="258" t="s">
         <v>54</v>
       </c>
       <c r="G15" t="str">
@@ -30396,19 +30450,19 @@
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A16" s="259" t="s">
+      <c r="A16" s="258" t="s">
         <v>124</v>
       </c>
-      <c r="B16" s="259" t="s">
+      <c r="B16" s="258" t="s">
         <v>126</v>
       </c>
-      <c r="C16" s="259" t="s">
+      <c r="C16" s="258" t="s">
         <v>125</v>
       </c>
-      <c r="D16" s="259">
-        <v>2</v>
-      </c>
-      <c r="E16" s="259" t="s">
+      <c r="D16" s="258">
+        <v>2</v>
+      </c>
+      <c r="E16" s="258" t="s">
         <v>51</v>
       </c>
       <c r="G16" t="str">
@@ -30428,19 +30482,19 @@
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A17" s="259" t="s">
+      <c r="A17" s="258" t="s">
         <v>124</v>
       </c>
-      <c r="B17" s="259" t="s">
+      <c r="B17" s="258" t="s">
         <v>126</v>
       </c>
-      <c r="C17" s="259" t="s">
+      <c r="C17" s="258" t="s">
         <v>125</v>
       </c>
-      <c r="D17" s="259">
-        <v>2</v>
-      </c>
-      <c r="E17" s="259" t="s">
+      <c r="D17" s="258">
+        <v>2</v>
+      </c>
+      <c r="E17" s="258" t="s">
         <v>364</v>
       </c>
       <c r="G17" t="str">
@@ -30460,19 +30514,19 @@
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A18" s="259" t="s">
+      <c r="A18" s="258" t="s">
         <v>413</v>
       </c>
-      <c r="B18" s="259" t="s">
+      <c r="B18" s="258" t="s">
         <v>412</v>
       </c>
-      <c r="C18" s="259" t="s">
+      <c r="C18" s="258" t="s">
         <v>414</v>
       </c>
-      <c r="D18" s="259">
-        <v>2</v>
-      </c>
-      <c r="E18" s="259" t="s">
+      <c r="D18" s="258">
+        <v>2</v>
+      </c>
+      <c r="E18" s="258" t="s">
         <v>415</v>
       </c>
       <c r="G18" t="str">
@@ -30492,19 +30546,19 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19" s="259" t="s">
+      <c r="A19" s="258" t="s">
         <v>413</v>
       </c>
-      <c r="B19" s="259" t="s">
+      <c r="B19" s="258" t="s">
         <v>141</v>
       </c>
-      <c r="C19" s="259" t="s">
+      <c r="C19" s="258" t="s">
         <v>414</v>
       </c>
-      <c r="D19" s="259">
-        <v>2</v>
-      </c>
-      <c r="E19" s="259" t="s">
+      <c r="D19" s="258">
+        <v>2</v>
+      </c>
+      <c r="E19" s="258" t="s">
         <v>426</v>
       </c>
       <c r="G19" t="str">
@@ -30524,19 +30578,19 @@
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20" s="259" t="s">
+      <c r="A20" s="258" t="s">
         <v>152</v>
       </c>
-      <c r="B20" s="259" t="s">
+      <c r="B20" s="258" t="s">
         <v>154</v>
       </c>
-      <c r="C20" s="259" t="s">
+      <c r="C20" s="258" t="s">
         <v>245</v>
       </c>
-      <c r="D20" s="259">
-        <v>2</v>
-      </c>
-      <c r="E20" s="259" t="s">
+      <c r="D20" s="258">
+        <v>2</v>
+      </c>
+      <c r="E20" s="258" t="s">
         <v>47</v>
       </c>
       <c r="G20" t="str">
@@ -30556,19 +30610,19 @@
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A21" s="259" t="s">
+      <c r="A21" s="258" t="s">
         <v>152</v>
       </c>
-      <c r="B21" s="259" t="s">
+      <c r="B21" s="258" t="s">
         <v>154</v>
       </c>
-      <c r="C21" s="259" t="s">
+      <c r="C21" s="258" t="s">
         <v>245</v>
       </c>
-      <c r="D21" s="259">
-        <v>2</v>
-      </c>
-      <c r="E21" s="259" t="s">
+      <c r="D21" s="258">
+        <v>2</v>
+      </c>
+      <c r="E21" s="258" t="s">
         <v>325</v>
       </c>
       <c r="G21" t="str">
@@ -30588,19 +30642,19 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A22" s="259" t="s">
+      <c r="A22" s="258" t="s">
         <v>152</v>
       </c>
-      <c r="B22" s="259" t="s">
+      <c r="B22" s="258" t="s">
         <v>154</v>
       </c>
-      <c r="C22" s="259" t="s">
+      <c r="C22" s="258" t="s">
         <v>245</v>
       </c>
-      <c r="D22" s="259">
-        <v>2</v>
-      </c>
-      <c r="E22" s="259" t="s">
+      <c r="D22" s="258">
+        <v>2</v>
+      </c>
+      <c r="E22" s="258" t="s">
         <v>188</v>
       </c>
       <c r="G22" t="str">
@@ -30620,19 +30674,19 @@
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A23" s="259" t="s">
+      <c r="A23" s="258" t="s">
         <v>152</v>
       </c>
-      <c r="B23" s="259" t="s">
+      <c r="B23" s="258" t="s">
         <v>154</v>
       </c>
-      <c r="C23" s="259" t="s">
+      <c r="C23" s="258" t="s">
         <v>153</v>
       </c>
-      <c r="D23" s="259">
-        <v>2</v>
-      </c>
-      <c r="E23" s="259" t="s">
+      <c r="D23" s="258">
+        <v>2</v>
+      </c>
+      <c r="E23" s="258" t="s">
         <v>155</v>
       </c>
       <c r="G23" t="str">
@@ -30652,19 +30706,19 @@
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A24" s="259" t="s">
+      <c r="A24" s="258" t="s">
         <v>336</v>
       </c>
-      <c r="B24" s="259" t="s">
+      <c r="B24" s="258" t="s">
         <v>338</v>
       </c>
-      <c r="C24" s="259" t="s">
+      <c r="C24" s="258" t="s">
         <v>337</v>
       </c>
-      <c r="D24" s="259">
-        <v>2</v>
-      </c>
-      <c r="E24" s="259" t="s">
+      <c r="D24" s="258">
+        <v>2</v>
+      </c>
+      <c r="E24" s="258" t="s">
         <v>286</v>
       </c>
       <c r="G24" t="str">
@@ -30684,19 +30738,19 @@
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A25" s="259" t="s">
+      <c r="A25" s="258" t="s">
         <v>336</v>
       </c>
-      <c r="B25" s="259" t="s">
+      <c r="B25" s="258" t="s">
         <v>338</v>
       </c>
-      <c r="C25" s="259" t="s">
+      <c r="C25" s="258" t="s">
         <v>337</v>
       </c>
-      <c r="D25" s="259">
-        <v>2</v>
-      </c>
-      <c r="E25" s="259">
+      <c r="D25" s="258">
+        <v>2</v>
+      </c>
+      <c r="E25" s="258">
         <v>0</v>
       </c>
       <c r="G25" t="str">
@@ -30716,19 +30770,19 @@
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A26" s="259" t="s">
+      <c r="A26" s="258" t="s">
         <v>111</v>
       </c>
-      <c r="B26" s="259" t="s">
+      <c r="B26" s="258" t="s">
         <v>416</v>
       </c>
-      <c r="C26" s="259" t="s">
+      <c r="C26" s="258" t="s">
         <v>112</v>
       </c>
-      <c r="D26" s="259">
-        <v>2</v>
-      </c>
-      <c r="E26" s="259" t="s">
+      <c r="D26" s="258">
+        <v>2</v>
+      </c>
+      <c r="E26" s="258" t="s">
         <v>102</v>
       </c>
       <c r="G26" t="str">
@@ -30748,19 +30802,19 @@
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A27" s="259" t="s">
+      <c r="A27" s="258" t="s">
         <v>111</v>
       </c>
-      <c r="B27" s="259" t="s">
+      <c r="B27" s="258" t="s">
         <v>416</v>
       </c>
-      <c r="C27" s="259" t="s">
+      <c r="C27" s="258" t="s">
         <v>112</v>
       </c>
-      <c r="D27" s="259">
-        <v>2</v>
-      </c>
-      <c r="E27" s="259" t="s">
+      <c r="D27" s="258">
+        <v>2</v>
+      </c>
+      <c r="E27" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G27" t="str">
@@ -30780,19 +30834,19 @@
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A28" s="259" t="s">
+      <c r="A28" s="258" t="s">
         <v>111</v>
       </c>
-      <c r="B28" s="259" t="s">
+      <c r="B28" s="258" t="s">
         <v>416</v>
       </c>
-      <c r="C28" s="259" t="s">
+      <c r="C28" s="258" t="s">
         <v>112</v>
       </c>
-      <c r="D28" s="259">
-        <v>2</v>
-      </c>
-      <c r="E28" s="259" t="s">
+      <c r="D28" s="258">
+        <v>2</v>
+      </c>
+      <c r="E28" s="258" t="s">
         <v>285</v>
       </c>
       <c r="G28" t="str">
@@ -30812,19 +30866,19 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A29" s="259" t="s">
+      <c r="A29" s="258" t="s">
         <v>111</v>
       </c>
-      <c r="B29" s="259" t="s">
+      <c r="B29" s="258" t="s">
         <v>416</v>
       </c>
-      <c r="C29" s="259" t="s">
+      <c r="C29" s="258" t="s">
         <v>112</v>
       </c>
-      <c r="D29" s="259">
-        <v>2</v>
-      </c>
-      <c r="E29" s="259" t="s">
+      <c r="D29" s="258">
+        <v>2</v>
+      </c>
+      <c r="E29" s="258" t="s">
         <v>417</v>
       </c>
       <c r="G29" t="str">
@@ -30844,19 +30898,19 @@
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A30" s="259" t="s">
+      <c r="A30" s="258" t="s">
         <v>106</v>
       </c>
-      <c r="B30" s="259" t="s">
+      <c r="B30" s="258" t="s">
         <v>418</v>
       </c>
-      <c r="C30" s="259" t="s">
+      <c r="C30" s="258" t="s">
         <v>107</v>
       </c>
-      <c r="D30" s="259">
-        <v>2</v>
-      </c>
-      <c r="E30" s="259" t="s">
+      <c r="D30" s="258">
+        <v>2</v>
+      </c>
+      <c r="E30" s="258" t="s">
         <v>58</v>
       </c>
       <c r="G30" t="str">
@@ -30876,19 +30930,19 @@
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A31" s="259" t="s">
+      <c r="A31" s="258" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="259" t="s">
+      <c r="B31" s="258" t="s">
         <v>418</v>
       </c>
-      <c r="C31" s="259" t="s">
+      <c r="C31" s="258" t="s">
         <v>107</v>
       </c>
-      <c r="D31" s="259">
-        <v>2</v>
-      </c>
-      <c r="E31" s="259" t="s">
+      <c r="D31" s="258">
+        <v>2</v>
+      </c>
+      <c r="E31" s="258" t="s">
         <v>417</v>
       </c>
       <c r="G31" t="str">
@@ -30908,19 +30962,19 @@
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A32" s="259" t="s">
+      <c r="A32" s="258" t="s">
         <v>193</v>
       </c>
-      <c r="B32" s="259" t="s">
+      <c r="B32" s="258" t="s">
         <v>191</v>
       </c>
-      <c r="C32" s="259" t="s">
+      <c r="C32" s="258" t="s">
         <v>450</v>
       </c>
-      <c r="D32" s="259">
-        <v>2</v>
-      </c>
-      <c r="E32" s="259" t="s">
+      <c r="D32" s="258">
+        <v>2</v>
+      </c>
+      <c r="E32" s="258" t="s">
         <v>54</v>
       </c>
       <c r="G32" t="str">
@@ -30940,19 +30994,19 @@
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A33" s="259" t="s">
+      <c r="A33" s="258" t="s">
         <v>193</v>
       </c>
-      <c r="B33" s="259" t="s">
+      <c r="B33" s="258" t="s">
         <v>191</v>
       </c>
-      <c r="C33" s="259" t="s">
+      <c r="C33" s="258" t="s">
         <v>450</v>
       </c>
-      <c r="D33" s="259">
-        <v>2</v>
-      </c>
-      <c r="E33" s="259" t="s">
+      <c r="D33" s="258">
+        <v>2</v>
+      </c>
+      <c r="E33" s="258" t="s">
         <v>54</v>
       </c>
       <c r="G33" t="str">
@@ -30972,19 +31026,19 @@
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A34" s="259" t="s">
+      <c r="A34" s="258" t="s">
         <v>288</v>
       </c>
-      <c r="B34" s="259" t="s">
+      <c r="B34" s="258" t="s">
         <v>290</v>
       </c>
-      <c r="C34" s="259" t="s">
+      <c r="C34" s="258" t="s">
         <v>289</v>
       </c>
-      <c r="D34" s="259">
-        <v>2</v>
-      </c>
-      <c r="E34" s="259" t="s">
+      <c r="D34" s="258">
+        <v>2</v>
+      </c>
+      <c r="E34" s="258" t="s">
         <v>291</v>
       </c>
       <c r="G34" t="str">
@@ -31004,19 +31058,19 @@
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A35" s="259" t="s">
+      <c r="A35" s="258" t="s">
         <v>288</v>
       </c>
-      <c r="B35" s="259" t="s">
+      <c r="B35" s="258" t="s">
         <v>290</v>
       </c>
-      <c r="C35" s="259" t="s">
+      <c r="C35" s="258" t="s">
         <v>289</v>
       </c>
-      <c r="D35" s="259">
-        <v>2</v>
-      </c>
-      <c r="E35" s="259" t="s">
+      <c r="D35" s="258">
+        <v>2</v>
+      </c>
+      <c r="E35" s="258" t="s">
         <v>291</v>
       </c>
       <c r="G35" t="str">
@@ -31036,19 +31090,19 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A36" s="259" t="s">
+      <c r="A36" s="258" t="s">
         <v>288</v>
       </c>
-      <c r="B36" s="259" t="s">
+      <c r="B36" s="258" t="s">
         <v>290</v>
       </c>
-      <c r="C36" s="259" t="s">
+      <c r="C36" s="258" t="s">
         <v>289</v>
       </c>
-      <c r="D36" s="259">
-        <v>2</v>
-      </c>
-      <c r="E36" s="259" t="s">
+      <c r="D36" s="258">
+        <v>2</v>
+      </c>
+      <c r="E36" s="258" t="s">
         <v>60</v>
       </c>
       <c r="G36" t="str">
@@ -31068,19 +31122,19 @@
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A37" s="259" t="s">
+      <c r="A37" s="258" t="s">
         <v>98</v>
       </c>
-      <c r="B37" s="259" t="s">
+      <c r="B37" s="258" t="s">
         <v>100</v>
       </c>
-      <c r="C37" s="259" t="s">
+      <c r="C37" s="258" t="s">
         <v>99</v>
       </c>
-      <c r="D37" s="259">
+      <c r="D37" s="258">
         <v>1</v>
       </c>
-      <c r="E37" s="259" t="s">
+      <c r="E37" s="258" t="s">
         <v>102</v>
       </c>
       <c r="G37" t="str">
@@ -31100,19 +31154,19 @@
       </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A38" s="259" t="s">
+      <c r="A38" s="258" t="s">
         <v>98</v>
       </c>
-      <c r="B38" s="259" t="s">
+      <c r="B38" s="258" t="s">
         <v>100</v>
       </c>
-      <c r="C38" s="259" t="s">
+      <c r="C38" s="258" t="s">
         <v>99</v>
       </c>
-      <c r="D38" s="259">
+      <c r="D38" s="258">
         <v>1</v>
       </c>
-      <c r="E38" s="259" t="s">
+      <c r="E38" s="258" t="s">
         <v>54</v>
       </c>
       <c r="G38" t="str">
@@ -31132,19 +31186,19 @@
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A39" s="259" t="s">
+      <c r="A39" s="258" t="s">
         <v>98</v>
       </c>
-      <c r="B39" s="259" t="s">
+      <c r="B39" s="258" t="s">
         <v>100</v>
       </c>
-      <c r="C39" s="259" t="s">
+      <c r="C39" s="258" t="s">
         <v>99</v>
       </c>
-      <c r="D39" s="259">
+      <c r="D39" s="258">
         <v>1</v>
       </c>
-      <c r="E39" s="259" t="s">
+      <c r="E39" s="258" t="s">
         <v>51</v>
       </c>
       <c r="G39" t="str">
@@ -31164,19 +31218,19 @@
       </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A40" s="259" t="s">
+      <c r="A40" s="258" t="s">
         <v>303</v>
       </c>
-      <c r="B40" s="259" t="s">
+      <c r="B40" s="258" t="s">
         <v>305</v>
       </c>
-      <c r="C40" s="259" t="s">
+      <c r="C40" s="258" t="s">
         <v>304</v>
       </c>
-      <c r="D40" s="259">
-        <v>2</v>
-      </c>
-      <c r="E40" s="259" t="s">
+      <c r="D40" s="258">
+        <v>2</v>
+      </c>
+      <c r="E40" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G40" t="str">
@@ -31196,19 +31250,19 @@
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A41" s="259" t="s">
+      <c r="A41" s="258" t="s">
         <v>128</v>
       </c>
-      <c r="B41" s="259" t="s">
+      <c r="B41" s="258" t="s">
         <v>126</v>
       </c>
-      <c r="C41" s="259" t="s">
+      <c r="C41" s="258" t="s">
         <v>129</v>
       </c>
-      <c r="D41" s="259">
-        <v>2</v>
-      </c>
-      <c r="E41" s="259" t="s">
+      <c r="D41" s="258">
+        <v>2</v>
+      </c>
+      <c r="E41" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G41" t="str">
@@ -31228,19 +31282,19 @@
       </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A42" s="259" t="s">
+      <c r="A42" s="258" t="s">
         <v>128</v>
       </c>
-      <c r="B42" s="259" t="s">
+      <c r="B42" s="258" t="s">
         <v>126</v>
       </c>
-      <c r="C42" s="259" t="s">
+      <c r="C42" s="258" t="s">
         <v>129</v>
       </c>
-      <c r="D42" s="259">
-        <v>2</v>
-      </c>
-      <c r="E42" s="259" t="s">
+      <c r="D42" s="258">
+        <v>2</v>
+      </c>
+      <c r="E42" s="258" t="s">
         <v>364</v>
       </c>
       <c r="G42" t="str">
@@ -31260,19 +31314,19 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A43" s="259" t="s">
+      <c r="A43" s="258" t="s">
         <v>202</v>
       </c>
-      <c r="B43" s="259" t="s">
+      <c r="B43" s="258" t="s">
         <v>204</v>
       </c>
-      <c r="C43" s="259" t="s">
+      <c r="C43" s="258" t="s">
         <v>203</v>
       </c>
-      <c r="D43" s="259">
-        <v>2</v>
-      </c>
-      <c r="E43" s="259" t="s">
+      <c r="D43" s="258">
+        <v>2</v>
+      </c>
+      <c r="E43" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G43" t="str">
@@ -31292,19 +31346,19 @@
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A44" s="259" t="s">
+      <c r="A44" s="258" t="s">
         <v>202</v>
       </c>
-      <c r="B44" s="259" t="s">
+      <c r="B44" s="258" t="s">
         <v>204</v>
       </c>
-      <c r="C44" s="259" t="s">
+      <c r="C44" s="258" t="s">
         <v>203</v>
       </c>
-      <c r="D44" s="259">
-        <v>2</v>
-      </c>
-      <c r="E44" s="259" t="s">
+      <c r="D44" s="258">
+        <v>2</v>
+      </c>
+      <c r="E44" s="258" t="s">
         <v>285</v>
       </c>
       <c r="G44" t="str">
@@ -31324,19 +31378,19 @@
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A45" s="259" t="s">
+      <c r="A45" s="258" t="s">
         <v>225</v>
       </c>
-      <c r="B45" s="259" t="s">
+      <c r="B45" s="258" t="s">
         <v>227</v>
       </c>
-      <c r="C45" s="259" t="s">
+      <c r="C45" s="258" t="s">
         <v>226</v>
       </c>
-      <c r="D45" s="259">
-        <v>2</v>
-      </c>
-      <c r="E45" s="259" t="s">
+      <c r="D45" s="258">
+        <v>2</v>
+      </c>
+      <c r="E45" s="258" t="s">
         <v>54</v>
       </c>
       <c r="G45" t="str">
@@ -31356,19 +31410,19 @@
       </c>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A46" s="259" t="s">
+      <c r="A46" s="258" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="259" t="s">
+      <c r="B46" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="C46" s="259" t="s">
+      <c r="C46" s="258" t="s">
         <v>53</v>
       </c>
-      <c r="D46" s="259">
+      <c r="D46" s="258">
         <v>1</v>
       </c>
-      <c r="E46" s="259" t="s">
+      <c r="E46" s="258" t="s">
         <v>54</v>
       </c>
       <c r="G46" t="str">
@@ -31388,19 +31442,19 @@
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A47" s="259" t="s">
+      <c r="A47" s="258" t="s">
         <v>103</v>
       </c>
-      <c r="B47" s="259" t="s">
+      <c r="B47" s="258" t="s">
         <v>100</v>
       </c>
-      <c r="C47" s="259" t="s">
+      <c r="C47" s="258" t="s">
         <v>104</v>
       </c>
-      <c r="D47" s="259">
+      <c r="D47" s="258">
         <v>3</v>
       </c>
-      <c r="E47" s="259" t="s">
+      <c r="E47" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G47" t="str">
@@ -31420,19 +31474,19 @@
       </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A48" s="259" t="s">
+      <c r="A48" s="258" t="s">
         <v>103</v>
       </c>
-      <c r="B48" s="259" t="s">
+      <c r="B48" s="258" t="s">
         <v>100</v>
       </c>
-      <c r="C48" s="259" t="s">
+      <c r="C48" s="258" t="s">
         <v>104</v>
       </c>
-      <c r="D48" s="259">
+      <c r="D48" s="258">
         <v>3</v>
       </c>
-      <c r="E48" s="259" t="s">
+      <c r="E48" s="258" t="s">
         <v>240</v>
       </c>
       <c r="G48" t="str">
@@ -31452,19 +31506,19 @@
       </c>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A49" s="259" t="s">
+      <c r="A49" s="258" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="259" t="s">
+      <c r="B49" s="258" t="s">
         <v>100</v>
       </c>
-      <c r="C49" s="259" t="s">
+      <c r="C49" s="258" t="s">
         <v>104</v>
       </c>
-      <c r="D49" s="259">
+      <c r="D49" s="258">
         <v>3</v>
       </c>
-      <c r="E49" s="259" t="s">
+      <c r="E49" s="258" t="s">
         <v>287</v>
       </c>
       <c r="G49" t="str">
@@ -31484,19 +31538,19 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A50" s="259" t="s">
+      <c r="A50" s="258" t="s">
         <v>103</v>
       </c>
-      <c r="B50" s="259" t="s">
+      <c r="B50" s="258" t="s">
         <v>100</v>
       </c>
-      <c r="C50" s="259" t="s">
+      <c r="C50" s="258" t="s">
         <v>104</v>
       </c>
-      <c r="D50" s="259">
+      <c r="D50" s="258">
         <v>3</v>
       </c>
-      <c r="E50" s="259" t="s">
+      <c r="E50" s="258" t="s">
         <v>265</v>
       </c>
       <c r="G50" t="str">
@@ -31516,19 +31570,19 @@
       </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A51" s="259" t="s">
+      <c r="A51" s="258" t="s">
         <v>67</v>
       </c>
-      <c r="B51" s="259" t="s">
+      <c r="B51" s="258" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="259" t="s">
+      <c r="C51" s="258" t="s">
         <v>68</v>
       </c>
-      <c r="D51" s="259">
-        <v>2</v>
-      </c>
-      <c r="E51" s="259" t="s">
+      <c r="D51" s="258">
+        <v>2</v>
+      </c>
+      <c r="E51" s="258" t="s">
         <v>70</v>
       </c>
       <c r="G51" t="str">
@@ -31548,19 +31602,19 @@
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A52" s="259" t="s">
+      <c r="A52" s="258" t="s">
         <v>77</v>
       </c>
-      <c r="B52" s="259" t="s">
+      <c r="B52" s="258" t="s">
         <v>79</v>
       </c>
-      <c r="C52" s="259" t="s">
+      <c r="C52" s="258" t="s">
         <v>78</v>
       </c>
-      <c r="D52" s="259">
-        <v>2</v>
-      </c>
-      <c r="E52" s="259" t="s">
+      <c r="D52" s="258">
+        <v>2</v>
+      </c>
+      <c r="E52" s="258" t="s">
         <v>60</v>
       </c>
       <c r="G52" t="str">
@@ -31580,19 +31634,19 @@
       </c>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A53" s="259" t="s">
+      <c r="A53" s="258" t="s">
         <v>160</v>
       </c>
-      <c r="B53" s="259" t="s">
+      <c r="B53" s="258" t="s">
         <v>79</v>
       </c>
-      <c r="C53" s="259" t="s">
+      <c r="C53" s="258" t="s">
         <v>161</v>
       </c>
-      <c r="D53" s="259">
+      <c r="D53" s="258">
         <v>4</v>
       </c>
-      <c r="E53" s="259" t="s">
+      <c r="E53" s="258" t="s">
         <v>60</v>
       </c>
       <c r="G53" t="str">
@@ -31612,19 +31666,19 @@
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A54" s="259" t="s">
+      <c r="A54" s="258" t="s">
         <v>160</v>
       </c>
-      <c r="B54" s="259" t="s">
+      <c r="B54" s="258" t="s">
         <v>79</v>
       </c>
-      <c r="C54" s="259" t="s">
+      <c r="C54" s="258" t="s">
         <v>161</v>
       </c>
-      <c r="D54" s="259">
+      <c r="D54" s="258">
         <v>4</v>
       </c>
-      <c r="E54" s="259" t="s">
+      <c r="E54" s="258" t="s">
         <v>285</v>
       </c>
       <c r="G54" t="str">
@@ -31644,19 +31698,19 @@
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A55" s="259" t="s">
+      <c r="A55" s="258" t="s">
         <v>160</v>
       </c>
-      <c r="B55" s="259" t="s">
+      <c r="B55" s="258" t="s">
         <v>399</v>
       </c>
-      <c r="C55" s="259" t="s">
+      <c r="C55" s="258" t="s">
         <v>161</v>
       </c>
-      <c r="D55" s="259">
+      <c r="D55" s="258">
         <v>4</v>
       </c>
-      <c r="E55" s="259" t="s">
+      <c r="E55" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G55" t="str">
@@ -31676,19 +31730,19 @@
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A56" s="259" t="s">
+      <c r="A56" s="258" t="s">
         <v>156</v>
       </c>
-      <c r="B56" s="259" t="s">
+      <c r="B56" s="258" t="s">
         <v>69</v>
       </c>
-      <c r="C56" s="259" t="s">
+      <c r="C56" s="258" t="s">
         <v>157</v>
       </c>
-      <c r="D56" s="259">
+      <c r="D56" s="258">
         <v>4</v>
       </c>
-      <c r="E56" s="259" t="s">
+      <c r="E56" s="258" t="s">
         <v>70</v>
       </c>
       <c r="G56" t="str">
@@ -31708,19 +31762,19 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A57" s="259" t="s">
+      <c r="A57" s="258" t="s">
         <v>263</v>
       </c>
-      <c r="B57" s="259" t="s">
+      <c r="B57" s="258" t="s">
         <v>231</v>
       </c>
-      <c r="C57" s="259" t="s">
+      <c r="C57" s="258" t="s">
         <v>264</v>
       </c>
-      <c r="D57" s="259">
-        <v>2</v>
-      </c>
-      <c r="E57" s="259" t="s">
+      <c r="D57" s="258">
+        <v>2</v>
+      </c>
+      <c r="E57" s="258" t="s">
         <v>265</v>
       </c>
       <c r="G57" t="str">
@@ -31740,19 +31794,19 @@
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A58" s="259" t="s">
+      <c r="A58" s="258" t="s">
         <v>263</v>
       </c>
-      <c r="B58" s="259" t="s">
+      <c r="B58" s="258" t="s">
         <v>231</v>
       </c>
-      <c r="C58" s="259" t="s">
+      <c r="C58" s="258" t="s">
         <v>264</v>
       </c>
-      <c r="D58" s="259">
-        <v>2</v>
-      </c>
-      <c r="E58" s="259" t="s">
+      <c r="D58" s="258">
+        <v>2</v>
+      </c>
+      <c r="E58" s="258" t="s">
         <v>329</v>
       </c>
       <c r="G58" t="str">
@@ -31772,19 +31826,19 @@
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A59" s="259" t="s">
+      <c r="A59" s="258" t="s">
         <v>251</v>
       </c>
-      <c r="B59" s="259" t="s">
+      <c r="B59" s="258" t="s">
         <v>302</v>
       </c>
-      <c r="C59" s="259" t="s">
+      <c r="C59" s="258" t="s">
         <v>252</v>
       </c>
-      <c r="D59" s="259">
+      <c r="D59" s="258">
         <v>0.5</v>
       </c>
-      <c r="E59" s="259" t="s">
+      <c r="E59" s="258" t="s">
         <v>30</v>
       </c>
       <c r="G59" t="str">
@@ -31804,19 +31858,19 @@
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A60" s="259" t="s">
+      <c r="A60" s="258" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="259" t="s">
+      <c r="B60" s="258" t="s">
         <v>76</v>
       </c>
-      <c r="C60" s="259" t="s">
+      <c r="C60" s="258" t="s">
         <v>75</v>
       </c>
-      <c r="D60" s="259">
+      <c r="D60" s="258">
         <v>3</v>
       </c>
-      <c r="E60" s="259" t="s">
+      <c r="E60" s="258" t="s">
         <v>60</v>
       </c>
       <c r="G60" t="str">
@@ -31836,19 +31890,19 @@
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A61" s="259" t="s">
+      <c r="A61" s="258" t="s">
         <v>212</v>
       </c>
-      <c r="B61" s="259" t="s">
+      <c r="B61" s="258" t="s">
         <v>214</v>
       </c>
-      <c r="C61" s="259" t="s">
+      <c r="C61" s="258" t="s">
         <v>213</v>
       </c>
-      <c r="D61" s="259">
-        <v>2</v>
-      </c>
-      <c r="E61" s="259" t="s">
+      <c r="D61" s="258">
+        <v>2</v>
+      </c>
+      <c r="E61" s="258" t="s">
         <v>215</v>
       </c>
       <c r="G61" t="str">
@@ -31868,19 +31922,19 @@
       </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A62" s="259" t="s">
+      <c r="A62" s="258" t="s">
         <v>376</v>
       </c>
-      <c r="B62" s="259" t="s">
+      <c r="B62" s="258" t="s">
         <v>378</v>
       </c>
-      <c r="C62" s="259" t="s">
+      <c r="C62" s="258" t="s">
         <v>377</v>
       </c>
-      <c r="D62" s="259">
+      <c r="D62" s="258">
         <v>4</v>
       </c>
-      <c r="E62" s="259" t="s">
+      <c r="E62" s="258" t="s">
         <v>60</v>
       </c>
       <c r="G62" t="str">
@@ -31900,19 +31954,19 @@
       </c>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A63" s="259" t="s">
+      <c r="A63" s="258" t="s">
         <v>216</v>
       </c>
-      <c r="B63" s="259" t="s">
+      <c r="B63" s="258" t="s">
         <v>214</v>
       </c>
-      <c r="C63" s="259" t="s">
+      <c r="C63" s="258" t="s">
         <v>217</v>
       </c>
-      <c r="D63" s="259">
+      <c r="D63" s="258">
         <v>1</v>
       </c>
-      <c r="E63" s="259" t="s">
+      <c r="E63" s="258" t="s">
         <v>215</v>
       </c>
       <c r="G63" t="str">
@@ -31932,19 +31986,19 @@
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A64" s="259" t="s">
+      <c r="A64" s="258" t="s">
         <v>216</v>
       </c>
-      <c r="B64" s="259" t="s">
+      <c r="B64" s="258" t="s">
         <v>214</v>
       </c>
-      <c r="C64" s="259" t="s">
+      <c r="C64" s="258" t="s">
         <v>217</v>
       </c>
-      <c r="D64" s="259">
+      <c r="D64" s="258">
         <v>1</v>
       </c>
-      <c r="E64" s="259" t="s">
+      <c r="E64" s="258" t="s">
         <v>54</v>
       </c>
       <c r="G64" t="str">
@@ -31964,19 +32018,19 @@
       </c>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A65" s="259" t="s">
+      <c r="A65" s="258" t="s">
         <v>243</v>
       </c>
-      <c r="B65" s="259" t="s">
+      <c r="B65" s="258" t="s">
         <v>154</v>
       </c>
-      <c r="C65" s="259" t="s">
+      <c r="C65" s="258" t="s">
         <v>244</v>
       </c>
-      <c r="D65" s="259">
-        <v>2</v>
-      </c>
-      <c r="E65" s="259" t="s">
+      <c r="D65" s="258">
+        <v>2</v>
+      </c>
+      <c r="E65" s="258" t="s">
         <v>54</v>
       </c>
       <c r="G65" t="str">
@@ -31996,19 +32050,19 @@
       </c>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A66" s="259" t="s">
+      <c r="A66" s="258" t="s">
         <v>248</v>
       </c>
-      <c r="B66" s="259" t="s">
+      <c r="B66" s="258" t="s">
         <v>302</v>
       </c>
-      <c r="C66" s="259" t="s">
+      <c r="C66" s="258" t="s">
         <v>249</v>
       </c>
-      <c r="D66" s="259">
-        <v>2</v>
-      </c>
-      <c r="E66" s="259" t="s">
+      <c r="D66" s="258">
+        <v>2</v>
+      </c>
+      <c r="E66" s="258" t="s">
         <v>285</v>
       </c>
       <c r="G66" t="str">
@@ -32028,19 +32082,19 @@
       </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A67" s="259" t="s">
+      <c r="A67" s="258" t="s">
         <v>248</v>
       </c>
-      <c r="B67" s="259" t="s">
+      <c r="B67" s="258" t="s">
         <v>302</v>
       </c>
-      <c r="C67" s="259" t="s">
+      <c r="C67" s="258" t="s">
         <v>249</v>
       </c>
-      <c r="D67" s="259">
-        <v>2</v>
-      </c>
-      <c r="E67" s="259" t="s">
+      <c r="D67" s="258">
+        <v>2</v>
+      </c>
+      <c r="E67" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G67" t="str">
@@ -32060,19 +32114,19 @@
       </c>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A68" s="259" t="s">
+      <c r="A68" s="258" t="s">
         <v>248</v>
       </c>
-      <c r="B68" s="259" t="s">
+      <c r="B68" s="258" t="s">
         <v>302</v>
       </c>
-      <c r="C68" s="259" t="s">
+      <c r="C68" s="258" t="s">
         <v>249</v>
       </c>
-      <c r="D68" s="259">
-        <v>2</v>
-      </c>
-      <c r="E68" s="259" t="s">
+      <c r="D68" s="258">
+        <v>2</v>
+      </c>
+      <c r="E68" s="258" t="s">
         <v>30</v>
       </c>
       <c r="G68" t="str">
@@ -32092,19 +32146,19 @@
       </c>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A69" s="259" t="s">
+      <c r="A69" s="258" t="s">
         <v>80</v>
       </c>
-      <c r="B69" s="259" t="s">
+      <c r="B69" s="258" t="s">
         <v>82</v>
       </c>
-      <c r="C69" s="259" t="s">
+      <c r="C69" s="258" t="s">
         <v>319</v>
       </c>
-      <c r="D69" s="259">
+      <c r="D69" s="258">
         <v>0.5</v>
       </c>
-      <c r="E69" s="259" t="s">
+      <c r="E69" s="258" t="s">
         <v>285</v>
       </c>
       <c r="G69" t="str">
@@ -32124,19 +32178,19 @@
       </c>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A70" s="259" t="s">
+      <c r="A70" s="258" t="s">
         <v>80</v>
       </c>
-      <c r="B70" s="259" t="s">
+      <c r="B70" s="258" t="s">
         <v>82</v>
       </c>
-      <c r="C70" s="259" t="s">
+      <c r="C70" s="258" t="s">
         <v>81</v>
       </c>
-      <c r="D70" s="259">
+      <c r="D70" s="258">
         <v>0.5</v>
       </c>
-      <c r="E70" s="259" t="s">
+      <c r="E70" s="258" t="s">
         <v>47</v>
       </c>
       <c r="G70" t="str">
@@ -32156,19 +32210,19 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A71" s="259" t="s">
+      <c r="A71" s="258" t="s">
         <v>131</v>
       </c>
-      <c r="B71" s="259" t="s">
+      <c r="B71" s="258" t="s">
         <v>133</v>
       </c>
-      <c r="C71" s="259" t="s">
+      <c r="C71" s="258" t="s">
         <v>132</v>
       </c>
-      <c r="D71" s="259">
+      <c r="D71" s="258">
         <v>1</v>
       </c>
-      <c r="E71" s="259" t="s">
+      <c r="E71" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G71" t="str">
@@ -32188,19 +32242,19 @@
       </c>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A72" s="259" t="s">
+      <c r="A72" s="258" t="s">
         <v>136</v>
       </c>
-      <c r="B72" s="259" t="s">
+      <c r="B72" s="258" t="s">
         <v>133</v>
       </c>
-      <c r="C72" s="259" t="s">
+      <c r="C72" s="258" t="s">
         <v>137</v>
       </c>
-      <c r="D72" s="259">
+      <c r="D72" s="258">
         <v>1</v>
       </c>
-      <c r="E72" s="259" t="s">
+      <c r="E72" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G72" t="str">
@@ -32220,19 +32274,19 @@
       </c>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A73" s="259" t="s">
+      <c r="A73" s="258" t="s">
         <v>136</v>
       </c>
-      <c r="B73" s="259" t="s">
+      <c r="B73" s="258" t="s">
         <v>133</v>
       </c>
-      <c r="C73" s="259" t="s">
+      <c r="C73" s="258" t="s">
         <v>137</v>
       </c>
-      <c r="D73" s="259">
-        <v>2</v>
-      </c>
-      <c r="E73" s="259" t="s">
+      <c r="D73" s="258">
+        <v>2</v>
+      </c>
+      <c r="E73" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G73" t="str">
@@ -32252,19 +32306,19 @@
       </c>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A74" s="259" t="s">
+      <c r="A74" s="258" t="s">
         <v>48</v>
       </c>
-      <c r="B74" s="259" t="s">
+      <c r="B74" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="C74" s="259" t="s">
+      <c r="C74" s="258" t="s">
         <v>49</v>
       </c>
-      <c r="D74" s="259">
-        <v>2</v>
-      </c>
-      <c r="E74" s="259" t="s">
+      <c r="D74" s="258">
+        <v>2</v>
+      </c>
+      <c r="E74" s="258" t="s">
         <v>51</v>
       </c>
       <c r="G74" t="str">
@@ -32284,19 +32338,19 @@
       </c>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A75" s="259" t="s">
+      <c r="A75" s="258" t="s">
         <v>48</v>
       </c>
-      <c r="B75" s="259" t="s">
+      <c r="B75" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="C75" s="259" t="s">
+      <c r="C75" s="258" t="s">
         <v>49</v>
       </c>
-      <c r="D75" s="259">
-        <v>2</v>
-      </c>
-      <c r="E75" s="259" t="s">
+      <c r="D75" s="258">
+        <v>2</v>
+      </c>
+      <c r="E75" s="258" t="s">
         <v>30</v>
       </c>
       <c r="G75" t="str">
@@ -32316,19 +32370,19 @@
       </c>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A76" s="259" t="s">
+      <c r="A76" s="258" t="s">
         <v>390</v>
       </c>
-      <c r="B76" s="259" t="s">
+      <c r="B76" s="258" t="s">
         <v>389</v>
       </c>
-      <c r="C76" s="259" t="s">
+      <c r="C76" s="258" t="s">
         <v>391</v>
       </c>
-      <c r="D76" s="259">
+      <c r="D76" s="258">
         <v>3</v>
       </c>
-      <c r="E76" s="259" t="s">
+      <c r="E76" s="258" t="s">
         <v>392</v>
       </c>
       <c r="G76" t="str">
@@ -32348,19 +32402,19 @@
       </c>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A77" s="259" t="s">
+      <c r="A77" s="258" t="s">
         <v>331</v>
       </c>
-      <c r="B77" s="259" t="s">
+      <c r="B77" s="258" t="s">
         <v>57</v>
       </c>
-      <c r="C77" s="259" t="s">
+      <c r="C77" s="258" t="s">
         <v>332</v>
       </c>
-      <c r="D77" s="259">
+      <c r="D77" s="258">
         <v>1</v>
       </c>
-      <c r="E77" s="259" t="s">
+      <c r="E77" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G77" t="str">
@@ -32380,19 +32434,19 @@
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A78" s="259" t="s">
+      <c r="A78" s="258" t="s">
         <v>383</v>
       </c>
-      <c r="B78" s="259" t="s">
+      <c r="B78" s="258" t="s">
         <v>385</v>
       </c>
-      <c r="C78" s="259" t="s">
+      <c r="C78" s="258" t="s">
         <v>384</v>
       </c>
-      <c r="D78" s="259">
+      <c r="D78" s="258">
         <v>3</v>
       </c>
-      <c r="E78" s="259" t="s">
+      <c r="E78" s="258" t="s">
         <v>215</v>
       </c>
       <c r="G78" t="str">
@@ -32412,19 +32466,19 @@
       </c>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A79" s="259" t="s">
+      <c r="A79" s="258" t="s">
         <v>322</v>
       </c>
-      <c r="B79" s="259" t="s">
+      <c r="B79" s="258" t="s">
         <v>324</v>
       </c>
-      <c r="C79" s="259" t="s">
+      <c r="C79" s="258" t="s">
         <v>323</v>
       </c>
-      <c r="D79" s="259">
+      <c r="D79" s="258">
         <v>1</v>
       </c>
-      <c r="E79" s="259" t="s">
+      <c r="E79" s="258" t="s">
         <v>325</v>
       </c>
       <c r="G79" t="str">
@@ -32444,19 +32498,19 @@
       </c>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A80" s="259" t="s">
+      <c r="A80" s="258" t="s">
         <v>182</v>
       </c>
-      <c r="B80" s="259" t="s">
+      <c r="B80" s="258" t="s">
         <v>184</v>
       </c>
-      <c r="C80" s="259" t="s">
+      <c r="C80" s="258" t="s">
         <v>183</v>
       </c>
-      <c r="D80" s="259">
+      <c r="D80" s="258">
         <v>0.6</v>
       </c>
-      <c r="E80" s="259" t="s">
+      <c r="E80" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G80" t="str">
@@ -32476,19 +32530,19 @@
       </c>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A81" s="259" t="s">
+      <c r="A81" s="258" t="s">
         <v>439</v>
       </c>
-      <c r="B81" s="259" t="s">
+      <c r="B81" s="258" t="s">
         <v>199</v>
       </c>
-      <c r="C81" s="259" t="s">
+      <c r="C81" s="258" t="s">
         <v>440</v>
       </c>
-      <c r="D81" s="259">
+      <c r="D81" s="258">
         <v>0.5</v>
       </c>
-      <c r="E81" s="259" t="s">
+      <c r="E81" s="258" t="s">
         <v>41</v>
       </c>
       <c r="G81" t="str">
@@ -32508,19 +32562,19 @@
       </c>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A82" s="259" t="s">
+      <c r="A82" s="258" t="s">
         <v>270</v>
       </c>
-      <c r="B82" s="259" t="s">
+      <c r="B82" s="258" t="s">
         <v>38</v>
       </c>
-      <c r="C82" s="259" t="s">
+      <c r="C82" s="258" t="s">
         <v>271</v>
       </c>
-      <c r="D82" s="259">
-        <v>2</v>
-      </c>
-      <c r="E82" s="259" t="s">
+      <c r="D82" s="258">
+        <v>2</v>
+      </c>
+      <c r="E82" s="258" t="s">
         <v>70</v>
       </c>
       <c r="G82" t="str">
@@ -32540,19 +32594,19 @@
       </c>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A83" s="259" t="s">
+      <c r="A83" s="258" t="s">
         <v>333</v>
       </c>
-      <c r="B83" s="259" t="s">
+      <c r="B83" s="258" t="s">
         <v>302</v>
       </c>
-      <c r="C83" s="259" t="s">
+      <c r="C83" s="258" t="s">
         <v>334</v>
       </c>
-      <c r="D83" s="259">
+      <c r="D83" s="258">
         <v>0.5</v>
       </c>
-      <c r="E83" s="259" t="s">
+      <c r="E83" s="258" t="s">
         <v>329</v>
       </c>
       <c r="G83" t="str">
@@ -32572,19 +32626,19 @@
       </c>
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A84" s="259" t="s">
+      <c r="A84" s="258" t="s">
         <v>36</v>
       </c>
-      <c r="B84" s="259" t="s">
+      <c r="B84" s="258" t="s">
         <v>38</v>
       </c>
-      <c r="C84" s="259" t="s">
+      <c r="C84" s="258" t="s">
         <v>400</v>
       </c>
-      <c r="D84" s="259">
+      <c r="D84" s="258">
         <v>1</v>
       </c>
-      <c r="E84" s="259" t="s">
+      <c r="E84" s="258" t="s">
         <v>41</v>
       </c>
       <c r="G84" t="str">
@@ -32604,19 +32658,19 @@
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A85" s="259" t="s">
+      <c r="A85" s="258" t="s">
         <v>36</v>
       </c>
-      <c r="B85" s="259" t="s">
+      <c r="B85" s="258" t="s">
         <v>38</v>
       </c>
-      <c r="C85" s="259" t="s">
+      <c r="C85" s="258" t="s">
         <v>400</v>
       </c>
-      <c r="D85" s="259">
+      <c r="D85" s="258">
         <v>1</v>
       </c>
-      <c r="E85" s="259" t="s">
+      <c r="E85" s="258" t="s">
         <v>41</v>
       </c>
       <c r="G85" t="str">
@@ -32636,19 +32690,19 @@
       </c>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A86" s="259" t="s">
+      <c r="A86" s="258" t="s">
         <v>121</v>
       </c>
-      <c r="B86" s="259" t="s">
+      <c r="B86" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="C86" s="259" t="s">
+      <c r="C86" s="258" t="s">
         <v>122</v>
       </c>
-      <c r="D86" s="259">
+      <c r="D86" s="258">
         <v>4</v>
       </c>
-      <c r="E86" s="259" t="s">
+      <c r="E86" s="258" t="s">
         <v>60</v>
       </c>
       <c r="G86" t="str">
@@ -32668,19 +32722,19 @@
       </c>
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A87" s="259" t="s">
+      <c r="A87" s="258" t="s">
         <v>121</v>
       </c>
-      <c r="B87" s="259" t="s">
+      <c r="B87" s="258" t="s">
         <v>458</v>
       </c>
-      <c r="C87" s="259" t="s">
+      <c r="C87" s="258" t="s">
         <v>122</v>
       </c>
-      <c r="D87" s="259">
+      <c r="D87" s="258">
         <v>4</v>
       </c>
-      <c r="E87" s="259" t="s">
+      <c r="E87" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G87" t="str">
@@ -32700,19 +32754,19 @@
       </c>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A88" s="259" t="s">
+      <c r="A88" s="258" t="s">
         <v>115</v>
       </c>
-      <c r="B88" s="259" t="s">
+      <c r="B88" s="258" t="s">
         <v>389</v>
       </c>
-      <c r="C88" s="259" t="s">
+      <c r="C88" s="258" t="s">
         <v>116</v>
       </c>
-      <c r="D88" s="259">
-        <v>2</v>
-      </c>
-      <c r="E88" s="259" t="s">
+      <c r="D88" s="258">
+        <v>2</v>
+      </c>
+      <c r="E88" s="258" t="s">
         <v>41</v>
       </c>
       <c r="G88" t="str">
@@ -32732,19 +32786,19 @@
       </c>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A89" s="259" t="s">
+      <c r="A89" s="258" t="s">
         <v>115</v>
       </c>
-      <c r="B89" s="259" t="s">
+      <c r="B89" s="258" t="s">
         <v>389</v>
       </c>
-      <c r="C89" s="259" t="s">
+      <c r="C89" s="258" t="s">
         <v>116</v>
       </c>
-      <c r="D89" s="259">
-        <v>2</v>
-      </c>
-      <c r="E89" s="259" t="s">
+      <c r="D89" s="258">
+        <v>2</v>
+      </c>
+      <c r="E89" s="258" t="s">
         <v>41</v>
       </c>
       <c r="G89" t="str">
@@ -32764,19 +32818,19 @@
       </c>
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A90" s="259" t="s">
+      <c r="A90" s="258" t="s">
         <v>115</v>
       </c>
-      <c r="B90" s="259" t="s">
+      <c r="B90" s="258" t="s">
         <v>389</v>
       </c>
-      <c r="C90" s="259" t="s">
+      <c r="C90" s="258" t="s">
         <v>116</v>
       </c>
-      <c r="D90" s="259">
-        <v>2</v>
-      </c>
-      <c r="E90" s="259" t="s">
+      <c r="D90" s="258">
+        <v>2</v>
+      </c>
+      <c r="E90" s="258" t="s">
         <v>150</v>
       </c>
       <c r="G90" t="str">
@@ -32796,19 +32850,19 @@
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A91" s="259" t="s">
+      <c r="A91" s="258" t="s">
         <v>115</v>
       </c>
-      <c r="B91" s="259" t="s">
+      <c r="B91" s="258" t="s">
         <v>389</v>
       </c>
-      <c r="C91" s="259" t="s">
+      <c r="C91" s="258" t="s">
         <v>116</v>
       </c>
-      <c r="D91" s="259">
-        <v>2</v>
-      </c>
-      <c r="E91" s="259" t="s">
+      <c r="D91" s="258">
+        <v>2</v>
+      </c>
+      <c r="E91" s="258" t="s">
         <v>89</v>
       </c>
       <c r="G91" t="str">
@@ -32828,19 +32882,19 @@
       </c>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A92" s="259" t="s">
+      <c r="A92" s="258" t="s">
         <v>434</v>
       </c>
-      <c r="B92" s="259" t="s">
+      <c r="B92" s="258" t="s">
         <v>57</v>
       </c>
-      <c r="C92" s="259" t="s">
+      <c r="C92" s="258" t="s">
         <v>59</v>
       </c>
-      <c r="D92" s="259">
-        <v>2</v>
-      </c>
-      <c r="E92" s="259" t="s">
+      <c r="D92" s="258">
+        <v>2</v>
+      </c>
+      <c r="E92" s="258" t="s">
         <v>60</v>
       </c>
       <c r="G92" t="str">
@@ -32860,19 +32914,19 @@
       </c>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A93" s="259" t="s">
+      <c r="A93" s="258" t="s">
         <v>444</v>
       </c>
-      <c r="B93" s="259" t="s">
+      <c r="B93" s="258" t="s">
         <v>184</v>
       </c>
-      <c r="C93" s="259" t="s">
+      <c r="C93" s="258" t="s">
         <v>445</v>
       </c>
-      <c r="D93" s="259">
+      <c r="D93" s="258">
         <v>0.5</v>
       </c>
-      <c r="E93" s="259" t="s">
+      <c r="E93" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G93" t="str">
@@ -32892,19 +32946,19 @@
       </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A94" s="259" t="s">
+      <c r="A94" s="258" t="s">
         <v>428</v>
       </c>
-      <c r="B94" s="259" t="s">
+      <c r="B94" s="258" t="s">
         <v>50</v>
       </c>
-      <c r="C94" s="259" t="s">
+      <c r="C94" s="258" t="s">
         <v>429</v>
       </c>
-      <c r="D94" s="259">
-        <v>2</v>
-      </c>
-      <c r="E94" s="259" t="s">
+      <c r="D94" s="258">
+        <v>2</v>
+      </c>
+      <c r="E94" s="258" t="s">
         <v>417</v>
       </c>
       <c r="G94" t="str">
@@ -32924,19 +32978,19 @@
       </c>
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A95" s="259" t="s">
+      <c r="A95" s="258" t="s">
         <v>119</v>
       </c>
-      <c r="B95" s="259" t="s">
+      <c r="B95" s="258" t="s">
         <v>389</v>
       </c>
-      <c r="C95" s="259" t="s">
+      <c r="C95" s="258" t="s">
         <v>120</v>
       </c>
-      <c r="D95" s="259">
-        <v>2</v>
-      </c>
-      <c r="E95" s="259" t="s">
+      <c r="D95" s="258">
+        <v>2</v>
+      </c>
+      <c r="E95" s="258" t="s">
         <v>41</v>
       </c>
       <c r="G95" t="str">
@@ -32956,19 +33010,19 @@
       </c>
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A96" s="259" t="s">
+      <c r="A96" s="258" t="s">
         <v>119</v>
       </c>
-      <c r="B96" s="259" t="s">
+      <c r="B96" s="258" t="s">
         <v>389</v>
       </c>
-      <c r="C96" s="259" t="s">
+      <c r="C96" s="258" t="s">
         <v>120</v>
       </c>
-      <c r="D96" s="259">
-        <v>2</v>
-      </c>
-      <c r="E96" s="259" t="s">
+      <c r="D96" s="258">
+        <v>2</v>
+      </c>
+      <c r="E96" s="258" t="s">
         <v>41</v>
       </c>
       <c r="G96" t="str">
@@ -32988,19 +33042,19 @@
       </c>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A97" s="259" t="s">
+      <c r="A97" s="258" t="s">
         <v>119</v>
       </c>
-      <c r="B97" s="259" t="s">
+      <c r="B97" s="258" t="s">
         <v>389</v>
       </c>
-      <c r="C97" s="259" t="s">
+      <c r="C97" s="258" t="s">
         <v>120</v>
       </c>
-      <c r="D97" s="259">
-        <v>2</v>
-      </c>
-      <c r="E97" s="259" t="s">
+      <c r="D97" s="258">
+        <v>2</v>
+      </c>
+      <c r="E97" s="258" t="s">
         <v>89</v>
       </c>
       <c r="G97" t="str">
@@ -33020,19 +33074,19 @@
       </c>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A98" s="259" t="s">
+      <c r="A98" s="258" t="s">
         <v>195</v>
       </c>
-      <c r="B98" s="259" t="s">
+      <c r="B98" s="258" t="s">
         <v>69</v>
       </c>
-      <c r="C98" s="259" t="s">
+      <c r="C98" s="258" t="s">
         <v>196</v>
       </c>
-      <c r="D98" s="259">
-        <v>2</v>
-      </c>
-      <c r="E98" s="259" t="s">
+      <c r="D98" s="258">
+        <v>2</v>
+      </c>
+      <c r="E98" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G98" t="str">
@@ -33052,19 +33106,19 @@
       </c>
     </row>
     <row r="99" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A99" s="259" t="s">
+      <c r="A99" s="258" t="s">
         <v>205</v>
       </c>
-      <c r="B99" s="259" t="s">
+      <c r="B99" s="258" t="s">
         <v>207</v>
       </c>
-      <c r="C99" s="259" t="s">
+      <c r="C99" s="258" t="s">
         <v>206</v>
       </c>
-      <c r="D99" s="259">
+      <c r="D99" s="258">
         <v>1</v>
       </c>
-      <c r="E99" s="259" t="s">
+      <c r="E99" s="258" t="s">
         <v>54</v>
       </c>
       <c r="G99" t="str">
@@ -33084,19 +33138,19 @@
       </c>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A100" s="259" t="s">
+      <c r="A100" s="258" t="s">
         <v>208</v>
       </c>
-      <c r="B100" s="259" t="s">
+      <c r="B100" s="258" t="s">
         <v>207</v>
       </c>
-      <c r="C100" s="259" t="s">
+      <c r="C100" s="258" t="s">
         <v>209</v>
       </c>
-      <c r="D100" s="259">
+      <c r="D100" s="258">
         <v>1</v>
       </c>
-      <c r="E100" s="259" t="s">
+      <c r="E100" s="258" t="s">
         <v>54</v>
       </c>
       <c r="G100" t="str">
@@ -33116,19 +33170,19 @@
       </c>
     </row>
     <row r="101" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A101" s="259" t="s">
+      <c r="A101" s="258" t="s">
         <v>408</v>
       </c>
-      <c r="B101" s="259" t="s">
+      <c r="B101" s="258" t="s">
         <v>63</v>
       </c>
-      <c r="C101" s="259" t="s">
+      <c r="C101" s="258" t="s">
         <v>409</v>
       </c>
-      <c r="D101" s="259">
+      <c r="D101" s="258">
         <v>1</v>
       </c>
-      <c r="E101" s="259" t="s">
+      <c r="E101" s="258" t="s">
         <v>41</v>
       </c>
       <c r="G101" t="str">
@@ -33148,19 +33202,19 @@
       </c>
     </row>
     <row r="102" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A102" s="259" t="s">
+      <c r="A102" s="258" t="s">
         <v>306</v>
       </c>
-      <c r="B102" s="259" t="s">
+      <c r="B102" s="258" t="s">
         <v>308</v>
       </c>
-      <c r="C102" s="259" t="s">
+      <c r="C102" s="258" t="s">
         <v>307</v>
       </c>
-      <c r="D102" s="259">
-        <v>2</v>
-      </c>
-      <c r="E102" s="259" t="s">
+      <c r="D102" s="258">
+        <v>2</v>
+      </c>
+      <c r="E102" s="258" t="s">
         <v>105</v>
       </c>
       <c r="G102" t="str">
@@ -33180,19 +33234,19 @@
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A103" s="259" t="s">
+      <c r="A103" s="258" t="s">
         <v>61</v>
       </c>
-      <c r="B103" s="259" t="s">
+      <c r="B103" s="258" t="s">
         <v>63</v>
       </c>
-      <c r="C103" s="259" t="s">
+      <c r="C103" s="258" t="s">
         <v>62</v>
       </c>
-      <c r="D103" s="259">
-        <v>2</v>
-      </c>
-      <c r="E103" s="259" t="s">
+      <c r="D103" s="258">
+        <v>2</v>
+      </c>
+      <c r="E103" s="258" t="s">
         <v>41</v>
       </c>
       <c r="G103" t="str">
@@ -33212,19 +33266,19 @@
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A104" s="259" t="s">
+      <c r="A104" s="258" t="s">
         <v>61</v>
       </c>
-      <c r="B104" s="259" t="s">
+      <c r="B104" s="258" t="s">
         <v>63</v>
       </c>
-      <c r="C104" s="259" t="s">
+      <c r="C104" s="258" t="s">
         <v>62</v>
       </c>
-      <c r="D104" s="259">
-        <v>2</v>
-      </c>
-      <c r="E104" s="259" t="s">
+      <c r="D104" s="258">
+        <v>2</v>
+      </c>
+      <c r="E104" s="258" t="s">
         <v>89</v>
       </c>
       <c r="G104" t="str">
@@ -33244,19 +33298,19 @@
       </c>
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A105" s="259" t="s">
+      <c r="A105" s="258" t="s">
         <v>442</v>
       </c>
-      <c r="B105" s="259" t="s">
+      <c r="B105" s="258" t="s">
         <v>184</v>
       </c>
-      <c r="C105" s="259" t="s">
+      <c r="C105" s="258" t="s">
         <v>443</v>
       </c>
-      <c r="D105" s="259">
-        <v>2</v>
-      </c>
-      <c r="E105" s="259" t="s">
+      <c r="D105" s="258">
+        <v>2</v>
+      </c>
+      <c r="E105" s="258" t="s">
         <v>70</v>
       </c>
       <c r="G105">
@@ -33276,886 +33330,886 @@
       </c>
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A106" s="259" t="s">
+      <c r="A106" s="258" t="s">
         <v>185</v>
       </c>
-      <c r="B106" s="259" t="s">
+      <c r="B106" s="258" t="s">
         <v>187</v>
       </c>
-      <c r="C106" s="259" t="s">
+      <c r="C106" s="258" t="s">
         <v>186</v>
       </c>
-      <c r="D106" s="259">
+      <c r="D106" s="258">
         <v>4</v>
       </c>
-      <c r="E106" s="259" t="s">
+      <c r="E106" s="258" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A107" s="259" t="s">
+      <c r="A107" s="258" t="s">
         <v>185</v>
       </c>
-      <c r="B107" s="259" t="s">
+      <c r="B107" s="258" t="s">
         <v>187</v>
       </c>
-      <c r="C107" s="259" t="s">
+      <c r="C107" s="258" t="s">
         <v>186</v>
       </c>
-      <c r="D107" s="259">
+      <c r="D107" s="258">
         <v>4</v>
       </c>
-      <c r="E107" s="259" t="s">
+      <c r="E107" s="258" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A108" s="259" t="s">
+      <c r="A108" s="258" t="s">
         <v>185</v>
       </c>
-      <c r="B108" s="259" t="s">
+      <c r="B108" s="258" t="s">
         <v>187</v>
       </c>
-      <c r="C108" s="259" t="s">
+      <c r="C108" s="258" t="s">
         <v>186</v>
       </c>
-      <c r="D108" s="259">
+      <c r="D108" s="258">
         <v>4</v>
       </c>
-      <c r="E108" s="259" t="s">
+      <c r="E108" s="258" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A109" s="259" t="s">
+      <c r="A109" s="258" t="s">
         <v>197</v>
       </c>
-      <c r="B109" s="259" t="s">
+      <c r="B109" s="258" t="s">
         <v>199</v>
       </c>
-      <c r="C109" s="259" t="s">
+      <c r="C109" s="258" t="s">
         <v>198</v>
       </c>
-      <c r="D109" s="259">
+      <c r="D109" s="258">
         <v>1</v>
       </c>
-      <c r="E109" s="259" t="s">
+      <c r="E109" s="258" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A110" s="259" t="s">
+      <c r="A110" s="258" t="s">
         <v>200</v>
       </c>
-      <c r="B110" s="259" t="s">
+      <c r="B110" s="258" t="s">
         <v>199</v>
       </c>
-      <c r="C110" s="259" t="s">
+      <c r="C110" s="258" t="s">
         <v>201</v>
       </c>
-      <c r="D110" s="259">
+      <c r="D110" s="258">
         <v>1</v>
       </c>
-      <c r="E110" s="259" t="s">
+      <c r="E110" s="258" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A111" s="259" t="s">
+      <c r="A111" s="258" t="s">
         <v>361</v>
       </c>
-      <c r="B111" s="259" t="s">
+      <c r="B111" s="258" t="s">
         <v>363</v>
       </c>
-      <c r="C111" s="259" t="s">
+      <c r="C111" s="258" t="s">
         <v>362</v>
       </c>
-      <c r="D111" s="259">
-        <v>2</v>
-      </c>
-      <c r="E111" s="259" t="s">
+      <c r="D111" s="258">
+        <v>2</v>
+      </c>
+      <c r="E111" s="258" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A112" s="259" t="s">
+      <c r="A112" s="258" t="s">
         <v>361</v>
       </c>
-      <c r="B112" s="259" t="s">
+      <c r="B112" s="258" t="s">
         <v>363</v>
       </c>
-      <c r="C112" s="259" t="s">
+      <c r="C112" s="258" t="s">
         <v>362</v>
       </c>
-      <c r="D112" s="259">
-        <v>2</v>
-      </c>
-      <c r="E112" s="259" t="s">
+      <c r="D112" s="258">
+        <v>2</v>
+      </c>
+      <c r="E112" s="258" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A113" s="259" t="s">
+      <c r="A113" s="258" t="s">
         <v>365</v>
       </c>
-      <c r="B113" s="259" t="s">
+      <c r="B113" s="258" t="s">
         <v>363</v>
       </c>
-      <c r="C113" s="259" t="s">
+      <c r="C113" s="258" t="s">
         <v>366</v>
       </c>
-      <c r="D113" s="259">
-        <v>2</v>
-      </c>
-      <c r="E113" s="259" t="s">
+      <c r="D113" s="258">
+        <v>2</v>
+      </c>
+      <c r="E113" s="258" t="s">
         <v>364</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A114" s="259" t="s">
+      <c r="A114" s="258" t="s">
         <v>365</v>
       </c>
-      <c r="B114" s="259" t="s">
+      <c r="B114" s="258" t="s">
         <v>363</v>
       </c>
-      <c r="C114" s="259" t="s">
+      <c r="C114" s="258" t="s">
         <v>366</v>
       </c>
-      <c r="D114" s="259">
-        <v>2</v>
-      </c>
-      <c r="E114" s="259" t="s">
+      <c r="D114" s="258">
+        <v>2</v>
+      </c>
+      <c r="E114" s="258" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A115" s="259" t="s">
+      <c r="A115" s="258" t="s">
         <v>380</v>
       </c>
-      <c r="B115" s="259" t="s">
+      <c r="B115" s="258" t="s">
         <v>382</v>
       </c>
-      <c r="C115" s="259" t="s">
+      <c r="C115" s="258" t="s">
         <v>381</v>
       </c>
-      <c r="D115" s="259">
+      <c r="D115" s="258">
         <v>4</v>
       </c>
-      <c r="E115" s="259" t="s">
+      <c r="E115" s="258" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A116" s="259" t="s">
+      <c r="A116" s="258" t="s">
         <v>436</v>
       </c>
-      <c r="B116" s="259" t="s">
+      <c r="B116" s="258" t="s">
         <v>308</v>
       </c>
-      <c r="C116" s="259" t="s">
+      <c r="C116" s="258" t="s">
         <v>437</v>
       </c>
-      <c r="D116" s="259">
-        <v>2</v>
-      </c>
-      <c r="E116" s="259" t="s">
+      <c r="D116" s="258">
+        <v>2</v>
+      </c>
+      <c r="E116" s="258" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A117" s="259" t="s">
+      <c r="A117" s="258" t="s">
         <v>71</v>
       </c>
-      <c r="B117" s="259" t="s">
+      <c r="B117" s="258" t="s">
         <v>73</v>
       </c>
-      <c r="C117" s="259" t="s">
+      <c r="C117" s="258" t="s">
         <v>72</v>
       </c>
-      <c r="D117" s="259">
-        <v>2</v>
-      </c>
-      <c r="E117" s="259" t="s">
+      <c r="D117" s="258">
+        <v>2</v>
+      </c>
+      <c r="E117" s="258" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A118" s="259" t="s">
+      <c r="A118" s="258" t="s">
         <v>71</v>
       </c>
-      <c r="B118" s="259" t="s">
+      <c r="B118" s="258" t="s">
         <v>73</v>
       </c>
-      <c r="C118" s="259" t="s">
+      <c r="C118" s="258" t="s">
         <v>72</v>
       </c>
-      <c r="D118" s="259">
-        <v>2</v>
-      </c>
-      <c r="E118" s="259" t="s">
+      <c r="D118" s="258">
+        <v>2</v>
+      </c>
+      <c r="E118" s="258" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A119" s="259" t="s">
+      <c r="A119" s="258" t="s">
         <v>261</v>
       </c>
-      <c r="B119" s="259" t="s">
+      <c r="B119" s="258" t="s">
         <v>148</v>
       </c>
-      <c r="C119" s="259" t="s">
+      <c r="C119" s="258" t="s">
         <v>262</v>
       </c>
-      <c r="D119" s="259">
+      <c r="D119" s="258">
         <v>3</v>
       </c>
-      <c r="E119" s="259" t="s">
+      <c r="E119" s="258" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A120" s="259" t="s">
+      <c r="A120" s="258" t="s">
         <v>261</v>
       </c>
-      <c r="B120" s="259" t="s">
+      <c r="B120" s="258" t="s">
         <v>148</v>
       </c>
-      <c r="C120" s="259" t="s">
+      <c r="C120" s="258" t="s">
         <v>262</v>
       </c>
-      <c r="D120" s="259">
+      <c r="D120" s="258">
         <v>3</v>
       </c>
-      <c r="E120" s="259" t="s">
+      <c r="E120" s="258" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A121" s="259" t="s">
+      <c r="A121" s="258" t="s">
         <v>261</v>
       </c>
-      <c r="B121" s="259" t="s">
+      <c r="B121" s="258" t="s">
         <v>148</v>
       </c>
-      <c r="C121" s="259" t="s">
+      <c r="C121" s="258" t="s">
         <v>262</v>
       </c>
-      <c r="D121" s="259">
+      <c r="D121" s="258">
         <v>3</v>
       </c>
-      <c r="E121" s="259" t="s">
+      <c r="E121" s="258" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A122" s="259" t="s">
+      <c r="A122" s="258" t="s">
         <v>258</v>
       </c>
-      <c r="B122" s="259" t="s">
+      <c r="B122" s="258" t="s">
         <v>148</v>
       </c>
-      <c r="C122" s="259" t="s">
+      <c r="C122" s="258" t="s">
         <v>259</v>
       </c>
-      <c r="D122" s="259">
+      <c r="D122" s="258">
         <v>1</v>
       </c>
-      <c r="E122" s="259" t="s">
+      <c r="E122" s="258" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A123" s="259" t="s">
+      <c r="A123" s="258" t="s">
         <v>258</v>
       </c>
-      <c r="B123" s="259" t="s">
+      <c r="B123" s="258" t="s">
         <v>148</v>
       </c>
-      <c r="C123" s="259" t="s">
+      <c r="C123" s="258" t="s">
         <v>259</v>
       </c>
-      <c r="D123" s="259">
+      <c r="D123" s="258">
         <v>1</v>
       </c>
-      <c r="E123" s="259">
+      <c r="E123" s="258">
         <v>0</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A124" s="259" t="s">
+      <c r="A124" s="258" t="s">
         <v>358</v>
       </c>
-      <c r="B124" s="259" t="s">
+      <c r="B124" s="258" t="s">
         <v>148</v>
       </c>
-      <c r="C124" s="259" t="s">
+      <c r="C124" s="258" t="s">
         <v>359</v>
       </c>
-      <c r="D124" s="259">
+      <c r="D124" s="258">
         <v>1</v>
       </c>
-      <c r="E124" s="259">
+      <c r="E124" s="258">
         <v>0</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A125" s="259" t="s">
+      <c r="A125" s="258" t="s">
         <v>189</v>
       </c>
-      <c r="B125" s="259" t="s">
+      <c r="B125" s="258" t="s">
         <v>191</v>
       </c>
-      <c r="C125" s="259" t="s">
+      <c r="C125" s="258" t="s">
         <v>448</v>
       </c>
-      <c r="D125" s="259">
+      <c r="D125" s="258">
         <v>0.6</v>
       </c>
-      <c r="E125" s="259" t="s">
+      <c r="E125" s="258" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A126" s="259" t="s">
+      <c r="A126" s="258" t="s">
         <v>189</v>
       </c>
-      <c r="B126" s="259" t="s">
+      <c r="B126" s="258" t="s">
         <v>191</v>
       </c>
-      <c r="C126" s="259" t="s">
+      <c r="C126" s="258" t="s">
         <v>190</v>
       </c>
-      <c r="D126" s="259">
+      <c r="D126" s="258">
         <v>0.6</v>
       </c>
-      <c r="E126" s="259" t="s">
+      <c r="E126" s="258" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A127" s="259" t="s">
+      <c r="A127" s="258" t="s">
         <v>344</v>
       </c>
-      <c r="B127" s="259" t="s">
+      <c r="B127" s="258" t="s">
         <v>346</v>
       </c>
-      <c r="C127" s="259" t="s">
+      <c r="C127" s="258" t="s">
         <v>345</v>
       </c>
-      <c r="D127" s="259">
-        <v>2</v>
-      </c>
-      <c r="E127" s="259" t="s">
+      <c r="D127" s="258">
+        <v>2</v>
+      </c>
+      <c r="E127" s="258" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A128" s="259" t="s">
+      <c r="A128" s="258" t="s">
         <v>32</v>
       </c>
-      <c r="B128" s="259" t="s">
+      <c r="B128" s="258" t="s">
         <v>34</v>
       </c>
-      <c r="C128" s="259" t="s">
+      <c r="C128" s="258" t="s">
         <v>33</v>
       </c>
-      <c r="D128" s="259">
-        <v>2</v>
-      </c>
-      <c r="E128" s="259" t="s">
+      <c r="D128" s="258">
+        <v>2</v>
+      </c>
+      <c r="E128" s="258" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A129" s="259" t="s">
+      <c r="A129" s="258" t="s">
         <v>218</v>
       </c>
-      <c r="B129" s="259" t="s">
+      <c r="B129" s="258" t="s">
         <v>220</v>
       </c>
-      <c r="C129" s="259" t="s">
+      <c r="C129" s="258" t="s">
         <v>219</v>
       </c>
-      <c r="D129" s="259">
-        <v>2</v>
-      </c>
-      <c r="E129" s="259" t="s">
+      <c r="D129" s="258">
+        <v>2</v>
+      </c>
+      <c r="E129" s="258" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A130" s="259" t="s">
+      <c r="A130" s="258" t="s">
         <v>218</v>
       </c>
-      <c r="B130" s="259" t="s">
+      <c r="B130" s="258" t="s">
         <v>220</v>
       </c>
-      <c r="C130" s="259" t="s">
+      <c r="C130" s="258" t="s">
         <v>219</v>
       </c>
-      <c r="D130" s="259">
-        <v>2</v>
-      </c>
-      <c r="E130" s="259" t="s">
+      <c r="D130" s="258">
+        <v>2</v>
+      </c>
+      <c r="E130" s="258" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A131" s="259" t="s">
+      <c r="A131" s="258" t="s">
         <v>410</v>
       </c>
-      <c r="B131" s="259" t="s">
+      <c r="B131" s="258" t="s">
         <v>412</v>
       </c>
-      <c r="C131" s="259" t="s">
+      <c r="C131" s="258" t="s">
         <v>411</v>
       </c>
-      <c r="D131" s="259">
-        <v>2</v>
-      </c>
-      <c r="E131" s="259" t="s">
+      <c r="D131" s="258">
+        <v>2</v>
+      </c>
+      <c r="E131" s="258" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A132" s="259" t="s">
+      <c r="A132" s="258" t="s">
         <v>222</v>
       </c>
-      <c r="B132" s="259" t="s">
+      <c r="B132" s="258" t="s">
         <v>224</v>
       </c>
-      <c r="C132" s="259" t="s">
+      <c r="C132" s="258" t="s">
         <v>223</v>
       </c>
-      <c r="D132" s="259">
-        <v>2</v>
-      </c>
-      <c r="E132" s="259" t="s">
+      <c r="D132" s="258">
+        <v>2</v>
+      </c>
+      <c r="E132" s="258" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A133" s="259" t="s">
+      <c r="A133" s="258" t="s">
         <v>423</v>
       </c>
-      <c r="B133" s="259" t="s">
+      <c r="B133" s="258" t="s">
         <v>425</v>
       </c>
-      <c r="C133" s="259" t="s">
+      <c r="C133" s="258" t="s">
         <v>424</v>
       </c>
-      <c r="D133" s="259">
-        <v>2</v>
-      </c>
-      <c r="E133" s="259" t="s">
+      <c r="D133" s="258">
+        <v>2</v>
+      </c>
+      <c r="E133" s="258" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A134" s="259" t="s">
+      <c r="A134" s="258" t="s">
         <v>64</v>
       </c>
-      <c r="B134" s="259" t="s">
+      <c r="B134" s="258" t="s">
         <v>66</v>
       </c>
-      <c r="C134" s="259" t="s">
+      <c r="C134" s="258" t="s">
         <v>269</v>
       </c>
-      <c r="D134" s="259">
-        <v>2</v>
-      </c>
-      <c r="E134" s="259" t="s">
+      <c r="D134" s="258">
+        <v>2</v>
+      </c>
+      <c r="E134" s="258" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A135" s="259" t="s">
+      <c r="A135" s="258" t="s">
         <v>64</v>
       </c>
-      <c r="B135" s="259" t="s">
+      <c r="B135" s="258" t="s">
         <v>66</v>
       </c>
-      <c r="C135" s="259" t="s">
+      <c r="C135" s="258" t="s">
         <v>181</v>
       </c>
-      <c r="D135" s="259">
-        <v>2</v>
-      </c>
-      <c r="E135" s="259" t="s">
+      <c r="D135" s="258">
+        <v>2</v>
+      </c>
+      <c r="E135" s="258" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A136" s="259" t="s">
+      <c r="A136" s="258" t="s">
         <v>64</v>
       </c>
-      <c r="B136" s="259" t="s">
+      <c r="B136" s="258" t="s">
         <v>66</v>
       </c>
-      <c r="C136" s="259" t="s">
+      <c r="C136" s="258" t="s">
         <v>181</v>
       </c>
-      <c r="D136" s="259">
-        <v>2</v>
-      </c>
-      <c r="E136" s="259" t="s">
+      <c r="D136" s="258">
+        <v>2</v>
+      </c>
+      <c r="E136" s="258" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A137" s="259" t="s">
+      <c r="A137" s="258" t="s">
         <v>387</v>
       </c>
-      <c r="B137" s="259" t="s">
+      <c r="B137" s="258" t="s">
         <v>389</v>
       </c>
-      <c r="C137" s="259" t="s">
+      <c r="C137" s="258" t="s">
         <v>388</v>
       </c>
-      <c r="D137" s="259">
+      <c r="D137" s="258">
         <v>1</v>
       </c>
-      <c r="E137" s="259" t="s">
+      <c r="E137" s="258" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A138" s="259" t="s">
+      <c r="A138" s="258" t="s">
         <v>387</v>
       </c>
-      <c r="B138" s="259" t="s">
+      <c r="B138" s="258" t="s">
         <v>389</v>
       </c>
-      <c r="C138" s="259" t="s">
+      <c r="C138" s="258" t="s">
         <v>388</v>
       </c>
-      <c r="D138" s="259">
+      <c r="D138" s="258">
         <v>1</v>
       </c>
-      <c r="E138" s="259" t="s">
+      <c r="E138" s="258" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A139" s="259" t="s">
+      <c r="A139" s="258" t="s">
         <v>168</v>
       </c>
-      <c r="B139" s="259" t="s">
+      <c r="B139" s="258" t="s">
         <v>148</v>
       </c>
-      <c r="C139" s="259" t="s">
+      <c r="C139" s="258" t="s">
         <v>169</v>
       </c>
-      <c r="D139" s="259">
-        <v>2</v>
-      </c>
-      <c r="E139" s="259" t="s">
+      <c r="D139" s="258">
+        <v>2</v>
+      </c>
+      <c r="E139" s="258" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A140" s="259" t="s">
+      <c r="A140" s="258" t="s">
         <v>168</v>
       </c>
-      <c r="B140" s="259" t="s">
+      <c r="B140" s="258" t="s">
         <v>148</v>
       </c>
-      <c r="C140" s="259" t="s">
+      <c r="C140" s="258" t="s">
         <v>169</v>
       </c>
-      <c r="D140" s="259">
-        <v>2</v>
-      </c>
-      <c r="E140" s="259">
+      <c r="D140" s="258">
+        <v>2</v>
+      </c>
+      <c r="E140" s="258">
         <v>0</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A141" s="259" t="s">
+      <c r="A141" s="258" t="s">
         <v>171</v>
       </c>
-      <c r="B141" s="259" t="s">
+      <c r="B141" s="258" t="s">
         <v>148</v>
       </c>
-      <c r="C141" s="259" t="s">
+      <c r="C141" s="258" t="s">
         <v>172</v>
       </c>
-      <c r="D141" s="259">
-        <v>2</v>
-      </c>
-      <c r="E141" s="259" t="s">
+      <c r="D141" s="258">
+        <v>2</v>
+      </c>
+      <c r="E141" s="258" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A142" s="259" t="s">
+      <c r="A142" s="258" t="s">
         <v>171</v>
       </c>
-      <c r="B142" s="259" t="s">
+      <c r="B142" s="258" t="s">
         <v>170</v>
       </c>
-      <c r="C142" s="259" t="s">
+      <c r="C142" s="258" t="s">
         <v>172</v>
       </c>
-      <c r="D142" s="259">
-        <v>2</v>
-      </c>
-      <c r="E142" s="259" t="s">
+      <c r="D142" s="258">
+        <v>2</v>
+      </c>
+      <c r="E142" s="258" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A143" s="259" t="s">
+      <c r="A143" s="258" t="s">
         <v>146</v>
       </c>
-      <c r="B143" s="259" t="s">
+      <c r="B143" s="258" t="s">
         <v>148</v>
       </c>
-      <c r="C143" s="259" t="s">
+      <c r="C143" s="258" t="s">
         <v>147</v>
       </c>
-      <c r="D143" s="259">
-        <v>2</v>
-      </c>
-      <c r="E143" s="259" t="s">
+      <c r="D143" s="258">
+        <v>2</v>
+      </c>
+      <c r="E143" s="258" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A144" s="259" t="s">
+      <c r="A144" s="258" t="s">
         <v>146</v>
       </c>
-      <c r="B144" s="259" t="s">
+      <c r="B144" s="258" t="s">
         <v>170</v>
       </c>
-      <c r="C144" s="259" t="s">
+      <c r="C144" s="258" t="s">
         <v>147</v>
       </c>
-      <c r="D144" s="259">
-        <v>2</v>
-      </c>
-      <c r="E144" s="259" t="s">
+      <c r="D144" s="258">
+        <v>2</v>
+      </c>
+      <c r="E144" s="258" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A145" s="259" t="s">
+      <c r="A145" s="258" t="s">
         <v>86</v>
       </c>
-      <c r="B145" s="259" t="s">
+      <c r="B145" s="258" t="s">
         <v>88</v>
       </c>
-      <c r="C145" s="259" t="s">
+      <c r="C145" s="258" t="s">
         <v>87</v>
       </c>
-      <c r="D145" s="259">
+      <c r="D145" s="258">
         <v>3</v>
       </c>
-      <c r="E145" s="259" t="s">
+      <c r="E145" s="258" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A146" s="259" t="s">
+      <c r="A146" s="258" t="s">
         <v>256</v>
       </c>
-      <c r="B146" s="259" t="s">
+      <c r="B146" s="258" t="s">
         <v>76</v>
       </c>
-      <c r="C146" s="259" t="s">
+      <c r="C146" s="258" t="s">
         <v>257</v>
       </c>
-      <c r="D146" s="259">
+      <c r="D146" s="258">
         <v>3</v>
       </c>
-      <c r="E146" s="259" t="s">
+      <c r="E146" s="258" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A147" s="259" t="s">
+      <c r="A147" s="258" t="s">
         <v>229</v>
       </c>
-      <c r="B147" s="259" t="s">
+      <c r="B147" s="258" t="s">
         <v>231</v>
       </c>
-      <c r="C147" s="259" t="s">
+      <c r="C147" s="258" t="s">
         <v>230</v>
       </c>
-      <c r="D147" s="259">
+      <c r="D147" s="258">
         <v>3</v>
       </c>
-      <c r="E147" s="259" t="s">
+      <c r="E147" s="258" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A148" s="259" t="s">
+      <c r="A148" s="258" t="s">
         <v>350</v>
       </c>
-      <c r="B148" s="259" t="s">
+      <c r="B148" s="258" t="s">
         <v>352</v>
       </c>
-      <c r="C148" s="259" t="s">
+      <c r="C148" s="258" t="s">
         <v>351</v>
       </c>
-      <c r="D148" s="259">
-        <v>2</v>
-      </c>
-      <c r="E148" s="259" t="s">
+      <c r="D148" s="258">
+        <v>2</v>
+      </c>
+      <c r="E148" s="258" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A149" s="259" t="s">
+      <c r="A149" s="258" t="s">
         <v>310</v>
       </c>
-      <c r="B149" s="259" t="s">
+      <c r="B149" s="258" t="s">
         <v>154</v>
       </c>
-      <c r="C149" s="259" t="s">
+      <c r="C149" s="258" t="s">
         <v>311</v>
       </c>
-      <c r="D149" s="259">
+      <c r="D149" s="258">
         <v>4</v>
       </c>
-      <c r="E149" s="259" t="s">
+      <c r="E149" s="258" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A150" s="259" t="s">
+      <c r="A150" s="258" t="s">
         <v>23</v>
       </c>
-      <c r="B150" s="259" t="s">
+      <c r="B150" s="258" t="s">
         <v>25</v>
       </c>
-      <c r="C150" s="259" t="s">
+      <c r="C150" s="258" t="s">
         <v>267</v>
       </c>
-      <c r="D150" s="259">
-        <v>2</v>
-      </c>
-      <c r="E150" s="259" t="s">
+      <c r="D150" s="258">
+        <v>2</v>
+      </c>
+      <c r="E150" s="258" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A151" s="259" t="s">
+      <c r="A151" s="258" t="s">
         <v>23</v>
       </c>
-      <c r="B151" s="259" t="s">
+      <c r="B151" s="258" t="s">
         <v>25</v>
       </c>
-      <c r="C151" s="259" t="s">
+      <c r="C151" s="258" t="s">
         <v>267</v>
       </c>
-      <c r="D151" s="259">
-        <v>2</v>
-      </c>
-      <c r="E151" s="259" t="s">
+      <c r="D151" s="258">
+        <v>2</v>
+      </c>
+      <c r="E151" s="258" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A152" s="259" t="s">
+      <c r="A152" s="258" t="s">
         <v>298</v>
       </c>
-      <c r="B152" s="259" t="s">
+      <c r="B152" s="258" t="s">
         <v>300</v>
       </c>
-      <c r="C152" s="259" t="s">
+      <c r="C152" s="258" t="s">
         <v>299</v>
       </c>
-      <c r="D152" s="259">
-        <v>2</v>
-      </c>
-      <c r="E152" s="259" t="s">
+      <c r="D152" s="258">
+        <v>2</v>
+      </c>
+      <c r="E152" s="258" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A153" s="259" t="s">
+      <c r="A153" s="258" t="s">
         <v>298</v>
       </c>
-      <c r="B153" s="259" t="s">
+      <c r="B153" s="258" t="s">
         <v>300</v>
       </c>
-      <c r="C153" s="259" t="s">
+      <c r="C153" s="258" t="s">
         <v>301</v>
       </c>
-      <c r="D153" s="259">
-        <v>2</v>
-      </c>
-      <c r="E153" s="259" t="s">
+      <c r="D153" s="258">
+        <v>2</v>
+      </c>
+      <c r="E153" s="258" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A154" s="259" t="s">
+      <c r="A154" s="258" t="s">
         <v>404</v>
       </c>
-      <c r="B154" s="259" t="s">
+      <c r="B154" s="258" t="s">
         <v>34</v>
       </c>
-      <c r="C154" s="259" t="s">
+      <c r="C154" s="258" t="s">
         <v>405</v>
       </c>
-      <c r="D154" s="259">
-        <v>2</v>
-      </c>
-      <c r="E154" s="259" t="s">
+      <c r="D154" s="258">
+        <v>2</v>
+      </c>
+      <c r="E154" s="258" t="s">
         <v>406</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A155" s="259" t="s">
+      <c r="A155" s="258" t="s">
         <v>170</v>
       </c>
-      <c r="B155" s="259">
+      <c r="B155" s="258">
         <v>0</v>
       </c>
-      <c r="C155" s="259" t="s">
+      <c r="C155" s="258" t="s">
         <v>247</v>
       </c>
-      <c r="D155" s="259">
-        <v>2</v>
-      </c>
-      <c r="E155" s="259" t="s">
+      <c r="D155" s="258">
+        <v>2</v>
+      </c>
+      <c r="E155" s="258" t="s">
         <v>403</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A156" s="259" t="s">
+      <c r="A156" s="258" t="s">
         <v>170</v>
       </c>
-      <c r="B156" s="259" t="s">
+      <c r="B156" s="258" t="s">
         <v>348</v>
       </c>
-      <c r="C156" s="259" t="s">
+      <c r="C156" s="258" t="s">
         <v>347</v>
       </c>
-      <c r="D156" s="259">
+      <c r="D156" s="258">
         <v>1</v>
       </c>
-      <c r="E156" s="259" t="s">
+      <c r="E156" s="258" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A157" s="260" t="s">
+      <c r="A157" s="259" t="s">
         <v>170</v>
       </c>
-      <c r="B157" s="260" t="s">
+      <c r="B157" s="259" t="s">
         <v>348</v>
       </c>
-      <c r="C157" s="260" t="s">
+      <c r="C157" s="259" t="s">
         <v>349</v>
       </c>
-      <c r="D157" s="260">
+      <c r="D157" s="259">
         <v>1</v>
       </c>
-      <c r="E157" s="260" t="s">
+      <c r="E157" s="259" t="s">
         <v>105</v>
       </c>
     </row>
@@ -35699,7 +35753,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="261" t="s">
+      <c r="A1" s="260" t="s">
         <v>467</v>
       </c>
       <c r="B1" s="257" t="s">
@@ -35711,7 +35765,7 @@
       <c r="D1" s="257" t="s">
         <v>468</v>
       </c>
-      <c r="E1" s="262" t="s">
+      <c r="E1" s="261" t="s">
         <v>12</v>
       </c>
     </row>
@@ -37484,7 +37538,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
+    <sheetView workbookViewId="1">
       <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
@@ -37498,7 +37552,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="261" t="s">
+      <c r="A1" s="260" t="s">
         <v>467</v>
       </c>
       <c r="B1" s="257" t="s">
@@ -37510,13 +37564,13 @@
       <c r="D1" s="257" t="s">
         <v>468</v>
       </c>
-      <c r="E1" s="262" t="s">
+      <c r="E1" s="261" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="263" t="s">
+      <c r="F1" s="262" t="s">
         <v>463</v>
       </c>
-      <c r="G1" s="263" t="s">
+      <c r="G1" s="262" t="s">
         <v>464</v>
       </c>
     </row>
@@ -39282,7 +39336,7 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A4AD150-E98C-41D1-8136-1D1281219F0B}">
   <sheetPr codeName="Sheet9"/>
-  <dimension ref="A1:A57"/>
+  <dimension ref="A1:A55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
@@ -39393,7 +39447,7 @@
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="258" t="str">
+      <c r="A20" t="str">
         <v>Hammer and Newman</v>
       </c>
     </row>
@@ -39403,7 +39457,7 @@
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="258" t="str">
+      <c r="A22" t="str">
         <v>Jack Duggal</v>
       </c>
     </row>
@@ -39533,50 +39587,44 @@
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="258" t="str">
+      <c r="A48" t="str">
         <v>Sunny Faronbi</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="258" t="str">
+      <c r="A49" t="str">
         <v>TBD</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="258" t="str">
+      <c r="A50" t="str">
         <v>Teresa Lawrence</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="258" t="str">
+      <c r="A51" t="str">
         <v>Thomas Jarocki</v>
       </c>
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="258" t="str">
+      <c r="A52" t="str">
         <v>Tony Prensa</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="258" t="str">
+      <c r="A53" t="str">
         <v>Traci Duez</v>
       </c>
     </row>
     <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="258" t="str">
+      <c r="A54" t="str">
         <v>Tyson Rydl</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="258" t="str">
+      <c r="A55" t="str">
         <v>Vijay Verma</v>
       </c>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="258"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="258"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding a Dates.csv more familiar with user and one table with notes and TBD/hotels. Some problems now include the stats show 46/NaN, scrolling to the right is not easy, and the new dates don't show under configure days
</commit_message>
<xml_diff>
--- a/Data/Draft Files/PMI Provided Course List Edits.xlsx
+++ b/Data/Draft Files/PMI Provided Course List Edits.xlsx
@@ -8,10 +8,10 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Documents\SchedulePro\Data\Draft Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40A5947A-707C-43A1-AD2E-F1F943C4E354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DF2507-5162-4FE5-8040-B8268F08055A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-53445" yWindow="2265" windowWidth="23010" windowHeight="12210" tabRatio="882" firstSheet="2" activeTab="10" xr2:uid="{E7EE0092-2BA9-4A50-8785-723FB1934021}"/>
-    <workbookView xWindow="-53010" yWindow="2700" windowWidth="23010" windowHeight="12210" tabRatio="803" xr2:uid="{9F697EAD-8F97-428C-B497-BADBFF50374A}"/>
+    <workbookView xWindow="-53280" yWindow="3690" windowWidth="23010" windowHeight="12210" tabRatio="882" firstSheet="2" activeTab="10" xr2:uid="{E7EE0092-2BA9-4A50-8785-723FB1934021}"/>
+    <workbookView xWindow="-53745" yWindow="2430" windowWidth="23010" windowHeight="12210" tabRatio="803" xr2:uid="{9F697EAD-8F97-428C-B497-BADBFF50374A}"/>
   </bookViews>
   <sheets>
     <sheet name="Original Data" sheetId="1" r:id="rId1"/>
@@ -2014,7 +2014,7 @@
     <t>notes will be crucial for example half day saying 9 am to 1 pm</t>
   </si>
   <si>
-    <t>before giving to client reset change log to 0</t>
+    <t>before giving to client reset change log to blank</t>
   </si>
 </sst>
 </file>
@@ -4927,7 +4927,7 @@
       <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>